<commit_message>
Documentation on Validation and Transformation started. Data Structures updated and copied as ODS files, too.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomyV1.0.3_CHANGE_LOG.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomyV1.0.3_CHANGE_LOG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD-Steps\ESPD\dist\cl\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2318,7 +2318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R823"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12953,7 +12953,7 @@
         <v>31</v>
       </c>
       <c r="L410" s="8" t="str">
-        <f>CONCATENATE(IF(A410="","",CONCATENATE("C", A410)),IF(B410="","",CONCATENATE("/G",B410)),IF(C410="","",CONCATENATE("/R",C410)), IF(D410="","",CONCATENATE("/G",B410,".",D410)), IF(E410="","",CONCATENATE("/R",E410)), IF(F410="","",CONCATENATE("/G",B410,".",D410,".",F410)), IF(G410="","",CONCATENATE("/R",G410)), IF(H410="","",CONCATENATE("/G",B410,".",D410,".",F410,".",H410)), IF(I410="","",CONCATENATE("/R",I410)),IF(J410="","",CONCATENATE("/G",B410,".",D410,".",F410,".",H410, ".",J410)), IF(K410="","",CONCATENATE("/R",K410)))</f>
+        <f t="shared" ref="L410:L436" si="12">CONCATENATE(IF(A410="","",CONCATENATE("C", A410)),IF(B410="","",CONCATENATE("/G",B410)),IF(C410="","",CONCATENATE("/R",C410)), IF(D410="","",CONCATENATE("/G",B410,".",D410)), IF(E410="","",CONCATENATE("/R",E410)), IF(F410="","",CONCATENATE("/G",B410,".",D410,".",F410)), IF(G410="","",CONCATENATE("/R",G410)), IF(H410="","",CONCATENATE("/G",B410,".",D410,".",F410,".",H410)), IF(I410="","",CONCATENATE("/R",I410)),IF(J410="","",CONCATENATE("/G",B410,".",D410,".",F410,".",H410, ".",J410)), IF(K410="","",CONCATENATE("/R",K410)))</f>
         <v>C31</v>
       </c>
       <c r="M410" s="8" t="s">
@@ -12975,7 +12975,7 @@
         <v>1</v>
       </c>
       <c r="L411" t="str">
-        <f>CONCATENATE(IF(A411="","",CONCATENATE("C", A411)),IF(B411="","",CONCATENATE("/G",B411)),IF(C411="","",CONCATENATE("/R",C411)), IF(D411="","",CONCATENATE("/G",B411,".",D411)), IF(E411="","",CONCATENATE("/R",E411)), IF(F411="","",CONCATENATE("/G",B411,".",D411,".",F411)), IF(G411="","",CONCATENATE("/R",G411)), IF(H411="","",CONCATENATE("/G",B411,".",D411,".",F411,".",H411)), IF(I411="","",CONCATENATE("/R",I411)),IF(J411="","",CONCATENATE("/G",B411,".",D411,".",F411,".",H411, ".",J411)), IF(K411="","",CONCATENATE("/R",K411)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1</v>
       </c>
       <c r="M411" t="s">
@@ -12996,7 +12996,7 @@
         <v>1</v>
       </c>
       <c r="L412" s="13" t="str">
-        <f>CONCATENATE(IF(A412="","",CONCATENATE("C", A412)),IF(B412="","",CONCATENATE("/G",B412)),IF(C412="","",CONCATENATE("/R",C412)), IF(D412="","",CONCATENATE("/G",B412,".",D412)), IF(E412="","",CONCATENATE("/R",E412)), IF(F412="","",CONCATENATE("/G",B412,".",D412,".",F412)), IF(G412="","",CONCATENATE("/R",G412)), IF(H412="","",CONCATENATE("/G",B412,".",D412,".",F412,".",H412)), IF(I412="","",CONCATENATE("/R",I412)),IF(J412="","",CONCATENATE("/G",B412,".",D412,".",F412,".",H412, ".",J412)), IF(K412="","",CONCATENATE("/R",K412)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/R1</v>
       </c>
       <c r="M412" s="13" t="s">
@@ -13026,7 +13026,7 @@
         <v>1</v>
       </c>
       <c r="L413" s="13" t="str">
-        <f>CONCATENATE(IF(A413="","",CONCATENATE("C", A413)),IF(B413="","",CONCATENATE("/G",B413)),IF(C413="","",CONCATENATE("/R",C413)), IF(D413="","",CONCATENATE("/G",B413,".",D413)), IF(E413="","",CONCATENATE("/R",E413)), IF(F413="","",CONCATENATE("/G",B413,".",D413,".",F413)), IF(G413="","",CONCATENATE("/R",G413)), IF(H413="","",CONCATENATE("/G",B413,".",D413,".",F413,".",H413)), IF(I413="","",CONCATENATE("/R",I413)),IF(J413="","",CONCATENATE("/G",B413,".",D413,".",F413,".",H413, ".",J413)), IF(K413="","",CONCATENATE("/R",K413)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1</v>
       </c>
       <c r="M413" s="13" t="s">
@@ -13050,7 +13050,7 @@
         <v>1</v>
       </c>
       <c r="L414" s="6" t="str">
-        <f>CONCATENATE(IF(A414="","",CONCATENATE("C", A414)),IF(B414="","",CONCATENATE("/G",B414)),IF(C414="","",CONCATENATE("/R",C414)), IF(D414="","",CONCATENATE("/G",B414,".",D414)), IF(E414="","",CONCATENATE("/R",E414)), IF(F414="","",CONCATENATE("/G",B414,".",D414,".",F414)), IF(G414="","",CONCATENATE("/R",G414)), IF(H414="","",CONCATENATE("/G",B414,".",D414,".",F414,".",H414)), IF(I414="","",CONCATENATE("/R",I414)),IF(J414="","",CONCATENATE("/G",B414,".",D414,".",F414,".",H414, ".",J414)), IF(K414="","",CONCATENATE("/R",K414)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/R1</v>
       </c>
       <c r="M414" s="6" t="s">
@@ -13077,7 +13077,7 @@
         <v>2</v>
       </c>
       <c r="L415" s="6" t="str">
-        <f>CONCATENATE(IF(A415="","",CONCATENATE("C", A415)),IF(B415="","",CONCATENATE("/G",B415)),IF(C415="","",CONCATENATE("/R",C415)), IF(D415="","",CONCATENATE("/G",B415,".",D415)), IF(E415="","",CONCATENATE("/R",E415)), IF(F415="","",CONCATENATE("/G",B415,".",D415,".",F415)), IF(G415="","",CONCATENATE("/R",G415)), IF(H415="","",CONCATENATE("/G",B415,".",D415,".",F415,".",H415)), IF(I415="","",CONCATENATE("/R",I415)),IF(J415="","",CONCATENATE("/G",B415,".",D415,".",F415,".",H415, ".",J415)), IF(K415="","",CONCATENATE("/R",K415)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/R2</v>
       </c>
       <c r="M415" s="6" t="s">
@@ -13104,7 +13104,7 @@
         <v>1</v>
       </c>
       <c r="L416" s="13" t="str">
-        <f>CONCATENATE(IF(A416="","",CONCATENATE("C", A416)),IF(B416="","",CONCATENATE("/G",B416)),IF(C416="","",CONCATENATE("/R",C416)), IF(D416="","",CONCATENATE("/G",B416,".",D416)), IF(E416="","",CONCATENATE("/R",E416)), IF(F416="","",CONCATENATE("/G",B416,".",D416,".",F416)), IF(G416="","",CONCATENATE("/R",G416)), IF(H416="","",CONCATENATE("/G",B416,".",D416,".",F416,".",H416)), IF(I416="","",CONCATENATE("/R",I416)),IF(J416="","",CONCATENATE("/G",B416,".",D416,".",F416,".",H416, ".",J416)), IF(K416="","",CONCATENATE("/R",K416)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.1</v>
       </c>
       <c r="M416" s="13" t="s">
@@ -13134,7 +13134,7 @@
         <v>1</v>
       </c>
       <c r="L417" s="13" t="str">
-        <f>CONCATENATE(IF(A417="","",CONCATENATE("C", A417)),IF(B417="","",CONCATENATE("/G",B417)),IF(C417="","",CONCATENATE("/R",C417)), IF(D417="","",CONCATENATE("/G",B417,".",D417)), IF(E417="","",CONCATENATE("/R",E417)), IF(F417="","",CONCATENATE("/G",B417,".",D417,".",F417)), IF(G417="","",CONCATENATE("/R",G417)), IF(H417="","",CONCATENATE("/G",B417,".",D417,".",F417,".",H417)), IF(I417="","",CONCATENATE("/R",I417)),IF(J417="","",CONCATENATE("/G",B417,".",D417,".",F417,".",H417, ".",J417)), IF(K417="","",CONCATENATE("/R",K417)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.1/R1</v>
       </c>
       <c r="M417" s="13" t="s">
@@ -13167,7 +13167,7 @@
         <v>2</v>
       </c>
       <c r="L418" s="13" t="str">
-        <f>CONCATENATE(IF(A418="","",CONCATENATE("C", A418)),IF(B418="","",CONCATENATE("/G",B418)),IF(C418="","",CONCATENATE("/R",C418)), IF(D418="","",CONCATENATE("/G",B418,".",D418)), IF(E418="","",CONCATENATE("/R",E418)), IF(F418="","",CONCATENATE("/G",B418,".",D418,".",F418)), IF(G418="","",CONCATENATE("/R",G418)), IF(H418="","",CONCATENATE("/G",B418,".",D418,".",F418,".",H418)), IF(I418="","",CONCATENATE("/R",I418)),IF(J418="","",CONCATENATE("/G",B418,".",D418,".",F418,".",H418, ".",J418)), IF(K418="","",CONCATENATE("/R",K418)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.1/R2</v>
       </c>
       <c r="M418" s="13" t="s">
@@ -13197,7 +13197,7 @@
         <v>2</v>
       </c>
       <c r="L419" s="13" t="str">
-        <f>CONCATENATE(IF(A419="","",CONCATENATE("C", A419)),IF(B419="","",CONCATENATE("/G",B419)),IF(C419="","",CONCATENATE("/R",C419)), IF(D419="","",CONCATENATE("/G",B419,".",D419)), IF(E419="","",CONCATENATE("/R",E419)), IF(F419="","",CONCATENATE("/G",B419,".",D419,".",F419)), IF(G419="","",CONCATENATE("/R",G419)), IF(H419="","",CONCATENATE("/G",B419,".",D419,".",F419,".",H419)), IF(I419="","",CONCATENATE("/R",I419)),IF(J419="","",CONCATENATE("/G",B419,".",D419,".",F419,".",H419, ".",J419)), IF(K419="","",CONCATENATE("/R",K419)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.2</v>
       </c>
       <c r="M419" s="13" t="s">
@@ -13227,7 +13227,7 @@
         <v>1</v>
       </c>
       <c r="L420" s="13" t="str">
-        <f>CONCATENATE(IF(A420="","",CONCATENATE("C", A420)),IF(B420="","",CONCATENATE("/G",B420)),IF(C420="","",CONCATENATE("/R",C420)), IF(D420="","",CONCATENATE("/G",B420,".",D420)), IF(E420="","",CONCATENATE("/R",E420)), IF(F420="","",CONCATENATE("/G",B420,".",D420,".",F420)), IF(G420="","",CONCATENATE("/R",G420)), IF(H420="","",CONCATENATE("/G",B420,".",D420,".",F420,".",H420)), IF(I420="","",CONCATENATE("/R",I420)),IF(J420="","",CONCATENATE("/G",B420,".",D420,".",F420,".",H420, ".",J420)), IF(K420="","",CONCATENATE("/R",K420)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.2/R1</v>
       </c>
       <c r="M420" s="13" t="s">
@@ -13260,7 +13260,7 @@
         <v>2</v>
       </c>
       <c r="L421" s="13" t="str">
-        <f>CONCATENATE(IF(A421="","",CONCATENATE("C", A421)),IF(B421="","",CONCATENATE("/G",B421)),IF(C421="","",CONCATENATE("/R",C421)), IF(D421="","",CONCATENATE("/G",B421,".",D421)), IF(E421="","",CONCATENATE("/R",E421)), IF(F421="","",CONCATENATE("/G",B421,".",D421,".",F421)), IF(G421="","",CONCATENATE("/R",G421)), IF(H421="","",CONCATENATE("/G",B421,".",D421,".",F421,".",H421)), IF(I421="","",CONCATENATE("/R",I421)),IF(J421="","",CONCATENATE("/G",B421,".",D421,".",F421,".",H421, ".",J421)), IF(K421="","",CONCATENATE("/R",K421)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.2/R2</v>
       </c>
       <c r="M421" s="13" t="s">
@@ -13290,7 +13290,7 @@
         <v>3</v>
       </c>
       <c r="L422" s="13" t="str">
-        <f>CONCATENATE(IF(A422="","",CONCATENATE("C", A422)),IF(B422="","",CONCATENATE("/G",B422)),IF(C422="","",CONCATENATE("/R",C422)), IF(D422="","",CONCATENATE("/G",B422,".",D422)), IF(E422="","",CONCATENATE("/R",E422)), IF(F422="","",CONCATENATE("/G",B422,".",D422,".",F422)), IF(G422="","",CONCATENATE("/R",G422)), IF(H422="","",CONCATENATE("/G",B422,".",D422,".",F422,".",H422)), IF(I422="","",CONCATENATE("/R",I422)),IF(J422="","",CONCATENATE("/G",B422,".",D422,".",F422,".",H422, ".",J422)), IF(K422="","",CONCATENATE("/R",K422)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.3</v>
       </c>
       <c r="M422" s="13" t="s">
@@ -13320,7 +13320,7 @@
         <v>1</v>
       </c>
       <c r="L423" s="13" t="str">
-        <f>CONCATENATE(IF(A423="","",CONCATENATE("C", A423)),IF(B423="","",CONCATENATE("/G",B423)),IF(C423="","",CONCATENATE("/R",C423)), IF(D423="","",CONCATENATE("/G",B423,".",D423)), IF(E423="","",CONCATENATE("/R",E423)), IF(F423="","",CONCATENATE("/G",B423,".",D423,".",F423)), IF(G423="","",CONCATENATE("/R",G423)), IF(H423="","",CONCATENATE("/G",B423,".",D423,".",F423,".",H423)), IF(I423="","",CONCATENATE("/R",I423)),IF(J423="","",CONCATENATE("/G",B423,".",D423,".",F423,".",H423, ".",J423)), IF(K423="","",CONCATENATE("/R",K423)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.3/R1</v>
       </c>
       <c r="M423" s="13" t="s">
@@ -13353,7 +13353,7 @@
         <v>2</v>
       </c>
       <c r="L424" s="13" t="str">
-        <f>CONCATENATE(IF(A424="","",CONCATENATE("C", A424)),IF(B424="","",CONCATENATE("/G",B424)),IF(C424="","",CONCATENATE("/R",C424)), IF(D424="","",CONCATENATE("/G",B424,".",D424)), IF(E424="","",CONCATENATE("/R",E424)), IF(F424="","",CONCATENATE("/G",B424,".",D424,".",F424)), IF(G424="","",CONCATENATE("/R",G424)), IF(H424="","",CONCATENATE("/G",B424,".",D424,".",F424,".",H424)), IF(I424="","",CONCATENATE("/R",I424)),IF(J424="","",CONCATENATE("/G",B424,".",D424,".",F424,".",H424, ".",J424)), IF(K424="","",CONCATENATE("/R",K424)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.3/R2</v>
       </c>
       <c r="M424" s="13" t="s">
@@ -13383,7 +13383,7 @@
         <v>4</v>
       </c>
       <c r="L425" s="13" t="str">
-        <f>CONCATENATE(IF(A425="","",CONCATENATE("C", A425)),IF(B425="","",CONCATENATE("/G",B425)),IF(C425="","",CONCATENATE("/R",C425)), IF(D425="","",CONCATENATE("/G",B425,".",D425)), IF(E425="","",CONCATENATE("/R",E425)), IF(F425="","",CONCATENATE("/G",B425,".",D425,".",F425)), IF(G425="","",CONCATENATE("/R",G425)), IF(H425="","",CONCATENATE("/G",B425,".",D425,".",F425,".",H425)), IF(I425="","",CONCATENATE("/R",I425)),IF(J425="","",CONCATENATE("/G",B425,".",D425,".",F425,".",H425, ".",J425)), IF(K425="","",CONCATENATE("/R",K425)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.4</v>
       </c>
       <c r="M425" s="13" t="s">
@@ -13413,7 +13413,7 @@
         <v>1</v>
       </c>
       <c r="L426" s="13" t="str">
-        <f>CONCATENATE(IF(A426="","",CONCATENATE("C", A426)),IF(B426="","",CONCATENATE("/G",B426)),IF(C426="","",CONCATENATE("/R",C426)), IF(D426="","",CONCATENATE("/G",B426,".",D426)), IF(E426="","",CONCATENATE("/R",E426)), IF(F426="","",CONCATENATE("/G",B426,".",D426,".",F426)), IF(G426="","",CONCATENATE("/R",G426)), IF(H426="","",CONCATENATE("/G",B426,".",D426,".",F426,".",H426)), IF(I426="","",CONCATENATE("/R",I426)),IF(J426="","",CONCATENATE("/G",B426,".",D426,".",F426,".",H426, ".",J426)), IF(K426="","",CONCATENATE("/R",K426)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.4/R1</v>
       </c>
       <c r="M426" s="13" t="s">
@@ -13446,7 +13446,7 @@
         <v>2</v>
       </c>
       <c r="L427" s="13" t="str">
-        <f>CONCATENATE(IF(A427="","",CONCATENATE("C", A427)),IF(B427="","",CONCATENATE("/G",B427)),IF(C427="","",CONCATENATE("/R",C427)), IF(D427="","",CONCATENATE("/G",B427,".",D427)), IF(E427="","",CONCATENATE("/R",E427)), IF(F427="","",CONCATENATE("/G",B427,".",D427,".",F427)), IF(G427="","",CONCATENATE("/R",G427)), IF(H427="","",CONCATENATE("/G",B427,".",D427,".",F427,".",H427)), IF(I427="","",CONCATENATE("/R",I427)),IF(J427="","",CONCATENATE("/G",B427,".",D427,".",F427,".",H427, ".",J427)), IF(K427="","",CONCATENATE("/R",K427)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.4/R2</v>
       </c>
       <c r="M427" s="13" t="s">
@@ -13476,7 +13476,7 @@
         <v>5</v>
       </c>
       <c r="L428" s="13" t="str">
-        <f>CONCATENATE(IF(A428="","",CONCATENATE("C", A428)),IF(B428="","",CONCATENATE("/G",B428)),IF(C428="","",CONCATENATE("/R",C428)), IF(D428="","",CONCATENATE("/G",B428,".",D428)), IF(E428="","",CONCATENATE("/R",E428)), IF(F428="","",CONCATENATE("/G",B428,".",D428,".",F428)), IF(G428="","",CONCATENATE("/R",G428)), IF(H428="","",CONCATENATE("/G",B428,".",D428,".",F428,".",H428)), IF(I428="","",CONCATENATE("/R",I428)),IF(J428="","",CONCATENATE("/G",B428,".",D428,".",F428,".",H428, ".",J428)), IF(K428="","",CONCATENATE("/R",K428)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.5</v>
       </c>
       <c r="M428" s="13" t="s">
@@ -13506,7 +13506,7 @@
         <v>1</v>
       </c>
       <c r="L429" s="13" t="str">
-        <f>CONCATENATE(IF(A429="","",CONCATENATE("C", A429)),IF(B429="","",CONCATENATE("/G",B429)),IF(C429="","",CONCATENATE("/R",C429)), IF(D429="","",CONCATENATE("/G",B429,".",D429)), IF(E429="","",CONCATENATE("/R",E429)), IF(F429="","",CONCATENATE("/G",B429,".",D429,".",F429)), IF(G429="","",CONCATENATE("/R",G429)), IF(H429="","",CONCATENATE("/G",B429,".",D429,".",F429,".",H429)), IF(I429="","",CONCATENATE("/R",I429)),IF(J429="","",CONCATENATE("/G",B429,".",D429,".",F429,".",H429, ".",J429)), IF(K429="","",CONCATENATE("/R",K429)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.5/R1</v>
       </c>
       <c r="M429" s="13" t="s">
@@ -13539,7 +13539,7 @@
         <v>2</v>
       </c>
       <c r="L430" s="13" t="str">
-        <f>CONCATENATE(IF(A430="","",CONCATENATE("C", A430)),IF(B430="","",CONCATENATE("/G",B430)),IF(C430="","",CONCATENATE("/R",C430)), IF(D430="","",CONCATENATE("/G",B430,".",D430)), IF(E430="","",CONCATENATE("/R",E430)), IF(F430="","",CONCATENATE("/G",B430,".",D430,".",F430)), IF(G430="","",CONCATENATE("/R",G430)), IF(H430="","",CONCATENATE("/G",B430,".",D430,".",F430,".",H430)), IF(I430="","",CONCATENATE("/R",I430)),IF(J430="","",CONCATENATE("/G",B430,".",D430,".",F430,".",H430, ".",J430)), IF(K430="","",CONCATENATE("/R",K430)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G1/G1.1/G1.1.5/R2</v>
       </c>
       <c r="M430" s="13" t="s">
@@ -13563,7 +13563,7 @@
         <v>2</v>
       </c>
       <c r="L431" t="str">
-        <f>CONCATENATE(IF(A431="","",CONCATENATE("C", A431)),IF(B431="","",CONCATENATE("/G",B431)),IF(C431="","",CONCATENATE("/R",C431)), IF(D431="","",CONCATENATE("/G",B431,".",D431)), IF(E431="","",CONCATENATE("/R",E431)), IF(F431="","",CONCATENATE("/G",B431,".",D431,".",F431)), IF(G431="","",CONCATENATE("/R",G431)), IF(H431="","",CONCATENATE("/G",B431,".",D431,".",F431,".",H431)), IF(I431="","",CONCATENATE("/R",I431)),IF(J431="","",CONCATENATE("/G",B431,".",D431,".",F431,".",H431, ".",J431)), IF(K431="","",CONCATENATE("/R",K431)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2</v>
       </c>
       <c r="M431" t="s">
@@ -13584,7 +13584,7 @@
         <v>1</v>
       </c>
       <c r="L432" t="str">
-        <f>CONCATENATE(IF(A432="","",CONCATENATE("C", A432)),IF(B432="","",CONCATENATE("/G",B432)),IF(C432="","",CONCATENATE("/R",C432)), IF(D432="","",CONCATENATE("/G",B432,".",D432)), IF(E432="","",CONCATENATE("/R",E432)), IF(F432="","",CONCATENATE("/G",B432,".",D432,".",F432)), IF(G432="","",CONCATENATE("/R",G432)), IF(H432="","",CONCATENATE("/G",B432,".",D432,".",F432,".",H432)), IF(I432="","",CONCATENATE("/R",I432)),IF(J432="","",CONCATENATE("/G",B432,".",D432,".",F432,".",H432, ".",J432)), IF(K432="","",CONCATENATE("/R",K432)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2/R1</v>
       </c>
       <c r="M432" t="s">
@@ -13611,7 +13611,7 @@
         <v>1</v>
       </c>
       <c r="L433" t="str">
-        <f>CONCATENATE(IF(A433="","",CONCATENATE("C", A433)),IF(B433="","",CONCATENATE("/G",B433)),IF(C433="","",CONCATENATE("/R",C433)), IF(D433="","",CONCATENATE("/G",B433,".",D433)), IF(E433="","",CONCATENATE("/R",E433)), IF(F433="","",CONCATENATE("/G",B433,".",D433,".",F433)), IF(G433="","",CONCATENATE("/R",G433)), IF(H433="","",CONCATENATE("/G",B433,".",D433,".",F433,".",H433)), IF(I433="","",CONCATENATE("/R",I433)),IF(J433="","",CONCATENATE("/G",B433,".",D433,".",F433,".",H433, ".",J433)), IF(K433="","",CONCATENATE("/R",K433)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2/G2.1</v>
       </c>
       <c r="M433" t="s">
@@ -13635,7 +13635,7 @@
         <v>1</v>
       </c>
       <c r="L434" t="str">
-        <f>CONCATENATE(IF(A434="","",CONCATENATE("C", A434)),IF(B434="","",CONCATENATE("/G",B434)),IF(C434="","",CONCATENATE("/R",C434)), IF(D434="","",CONCATENATE("/G",B434,".",D434)), IF(E434="","",CONCATENATE("/R",E434)), IF(F434="","",CONCATENATE("/G",B434,".",D434,".",F434)), IF(G434="","",CONCATENATE("/R",G434)), IF(H434="","",CONCATENATE("/G",B434,".",D434,".",F434,".",H434)), IF(I434="","",CONCATENATE("/R",I434)),IF(J434="","",CONCATENATE("/G",B434,".",D434,".",F434,".",H434, ".",J434)), IF(K434="","",CONCATENATE("/R",K434)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2/G2.1/R1</v>
       </c>
       <c r="M434" t="s">
@@ -13662,7 +13662,7 @@
         <v>2</v>
       </c>
       <c r="L435" t="str">
-        <f>CONCATENATE(IF(A435="","",CONCATENATE("C", A435)),IF(B435="","",CONCATENATE("/G",B435)),IF(C435="","",CONCATENATE("/R",C435)), IF(D435="","",CONCATENATE("/G",B435,".",D435)), IF(E435="","",CONCATENATE("/R",E435)), IF(F435="","",CONCATENATE("/G",B435,".",D435,".",F435)), IF(G435="","",CONCATENATE("/R",G435)), IF(H435="","",CONCATENATE("/G",B435,".",D435,".",F435,".",H435)), IF(I435="","",CONCATENATE("/R",I435)),IF(J435="","",CONCATENATE("/G",B435,".",D435,".",F435,".",H435, ".",J435)), IF(K435="","",CONCATENATE("/R",K435)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2/G2.1/R2</v>
       </c>
       <c r="M435" t="s">
@@ -13689,7 +13689,7 @@
         <v>3</v>
       </c>
       <c r="L436" s="6" t="str">
-        <f>CONCATENATE(IF(A436="","",CONCATENATE("C", A436)),IF(B436="","",CONCATENATE("/G",B436)),IF(C436="","",CONCATENATE("/R",C436)), IF(D436="","",CONCATENATE("/G",B436,".",D436)), IF(E436="","",CONCATENATE("/R",E436)), IF(F436="","",CONCATENATE("/G",B436,".",D436,".",F436)), IF(G436="","",CONCATENATE("/R",G436)), IF(H436="","",CONCATENATE("/G",B436,".",D436,".",F436,".",H436)), IF(I436="","",CONCATENATE("/R",I436)),IF(J436="","",CONCATENATE("/G",B436,".",D436,".",F436,".",H436, ".",J436)), IF(K436="","",CONCATENATE("/R",K436)))</f>
+        <f t="shared" si="12"/>
         <v>C31/G2/G2.1/R3</v>
       </c>
       <c r="M436" s="6" t="s">
@@ -13946,7 +13946,7 @@
         <v>1</v>
       </c>
       <c r="L445" s="13" t="str">
-        <f t="shared" ref="L445:L481" si="12">CONCATENATE(IF(A445="","",CONCATENATE("C", A445)),IF(B445="","",CONCATENATE("/G",B445)),IF(C445="","",CONCATENATE("/R",C445)), IF(D445="","",CONCATENATE("/G",B445,".",D445)), IF(E445="","",CONCATENATE("/R",E445)), IF(F445="","",CONCATENATE("/G",B445,".",D445,".",F445)), IF(G445="","",CONCATENATE("/R",G445)), IF(H445="","",CONCATENATE("/G",B445,".",D445,".",F445,".",H445)), IF(I445="","",CONCATENATE("/R",I445)),IF(J445="","",CONCATENATE("/G",B445,".",D445,".",F445,".",H445, ".",J445)), IF(K445="","",CONCATENATE("/R",K445)))</f>
+        <f t="shared" ref="L445:L481" si="13">CONCATENATE(IF(A445="","",CONCATENATE("C", A445)),IF(B445="","",CONCATENATE("/G",B445)),IF(C445="","",CONCATENATE("/R",C445)), IF(D445="","",CONCATENATE("/G",B445,".",D445)), IF(E445="","",CONCATENATE("/R",E445)), IF(F445="","",CONCATENATE("/G",B445,".",D445,".",F445)), IF(G445="","",CONCATENATE("/R",G445)), IF(H445="","",CONCATENATE("/G",B445,".",D445,".",F445,".",H445)), IF(I445="","",CONCATENATE("/R",I445)),IF(J445="","",CONCATENATE("/G",B445,".",D445,".",F445,".",H445, ".",J445)), IF(K445="","",CONCATENATE("/R",K445)))</f>
         <v>C32/G1/G1.1/G1.1.1</v>
       </c>
       <c r="M445" s="13" t="s">
@@ -13976,7 +13976,7 @@
         <v>1</v>
       </c>
       <c r="L446" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.1/R1</v>
       </c>
       <c r="M446" s="13" t="s">
@@ -14009,7 +14009,7 @@
         <v>2</v>
       </c>
       <c r="L447" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.1/R2</v>
       </c>
       <c r="M447" s="13" t="s">
@@ -14039,7 +14039,7 @@
         <v>2</v>
       </c>
       <c r="L448" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.2</v>
       </c>
       <c r="M448" s="13" t="s">
@@ -14069,7 +14069,7 @@
         <v>1</v>
       </c>
       <c r="L449" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.2/R1</v>
       </c>
       <c r="M449" s="13" t="s">
@@ -14102,7 +14102,7 @@
         <v>2</v>
       </c>
       <c r="L450" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.2/R2</v>
       </c>
       <c r="M450" s="13" t="s">
@@ -14132,7 +14132,7 @@
         <v>3</v>
       </c>
       <c r="L451" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.3</v>
       </c>
       <c r="M451" s="13" t="s">
@@ -14162,7 +14162,7 @@
         <v>1</v>
       </c>
       <c r="L452" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.3/R1</v>
       </c>
       <c r="M452" s="13" t="s">
@@ -14195,7 +14195,7 @@
         <v>2</v>
       </c>
       <c r="L453" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.3/R2</v>
       </c>
       <c r="M453" s="13" t="s">
@@ -14225,7 +14225,7 @@
         <v>4</v>
       </c>
       <c r="L454" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.4</v>
       </c>
       <c r="M454" s="13" t="s">
@@ -14255,7 +14255,7 @@
         <v>1</v>
       </c>
       <c r="L455" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.4/R1</v>
       </c>
       <c r="M455" s="13" t="s">
@@ -14288,7 +14288,7 @@
         <v>2</v>
       </c>
       <c r="L456" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.4/R2</v>
       </c>
       <c r="M456" s="13" t="s">
@@ -14318,7 +14318,7 @@
         <v>5</v>
       </c>
       <c r="L457" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.5</v>
       </c>
       <c r="M457" s="13" t="s">
@@ -14348,7 +14348,7 @@
         <v>1</v>
       </c>
       <c r="L458" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.5/R1</v>
       </c>
       <c r="M458" s="13" t="s">
@@ -14381,7 +14381,7 @@
         <v>2</v>
       </c>
       <c r="L459" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G1/G1.1/G1.1.5/R2</v>
       </c>
       <c r="M459" s="13" t="s">
@@ -14405,7 +14405,7 @@
         <v>2</v>
       </c>
       <c r="L460" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2</v>
       </c>
       <c r="M460" t="s">
@@ -14426,7 +14426,7 @@
         <v>1</v>
       </c>
       <c r="L461" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2/R1</v>
       </c>
       <c r="M461" t="s">
@@ -14453,7 +14453,7 @@
         <v>1</v>
       </c>
       <c r="L462" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2/G2.1</v>
       </c>
       <c r="M462" t="s">
@@ -14477,7 +14477,7 @@
         <v>1</v>
       </c>
       <c r="L463" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2/G2.1/R1</v>
       </c>
       <c r="M463" t="s">
@@ -14504,7 +14504,7 @@
         <v>2</v>
       </c>
       <c r="L464" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2/G2.1/R2</v>
       </c>
       <c r="M464" t="s">
@@ -14531,7 +14531,7 @@
         <v>3</v>
       </c>
       <c r="L465" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C32/G2/G2.1/R3</v>
       </c>
       <c r="M465" s="6" t="s">
@@ -14549,7 +14549,7 @@
         <v>33</v>
       </c>
       <c r="L466" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C33</v>
       </c>
       <c r="M466" s="8" t="s">
@@ -14571,7 +14571,7 @@
         <v>1</v>
       </c>
       <c r="L467" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C33/G1</v>
       </c>
       <c r="M467" t="s">
@@ -14592,7 +14592,7 @@
         <v>1</v>
       </c>
       <c r="L468" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C33/G1/R1</v>
       </c>
       <c r="M468" t="s">
@@ -14610,7 +14610,7 @@
         <v>34</v>
       </c>
       <c r="L469" s="8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34</v>
       </c>
       <c r="M469" s="8" t="s">
@@ -14634,7 +14634,7 @@
         <v>1</v>
       </c>
       <c r="L470" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1</v>
       </c>
       <c r="M470" s="13" t="s">
@@ -14658,7 +14658,7 @@
         <v>1</v>
       </c>
       <c r="L471" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/R1</v>
       </c>
       <c r="M471" s="13" t="s">
@@ -14682,7 +14682,7 @@
         <v>1</v>
       </c>
       <c r="L472" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1</v>
       </c>
       <c r="M472" t="s">
@@ -14709,7 +14709,7 @@
         <v>1</v>
       </c>
       <c r="L473" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/R1</v>
       </c>
       <c r="M473" t="s">
@@ -14736,7 +14736,7 @@
         <v>2</v>
       </c>
       <c r="L474" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/R2</v>
       </c>
       <c r="M474" t="s">
@@ -14763,7 +14763,7 @@
         <v>2</v>
       </c>
       <c r="L475" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.2</v>
       </c>
       <c r="M475" s="13" t="s">
@@ -14790,7 +14790,7 @@
         <v>1</v>
       </c>
       <c r="L476" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.2/R1</v>
       </c>
       <c r="M476" s="13" t="s">
@@ -14820,7 +14820,7 @@
         <v>2</v>
       </c>
       <c r="L477" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.2/R2</v>
       </c>
       <c r="M477" s="13" t="s">
@@ -14847,7 +14847,7 @@
         <v>3</v>
       </c>
       <c r="L478" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.3</v>
       </c>
       <c r="M478" s="13" t="s">
@@ -14874,7 +14874,7 @@
         <v>1</v>
       </c>
       <c r="L479" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.3/R1</v>
       </c>
       <c r="M479" s="13" t="s">
@@ -14904,7 +14904,7 @@
         <v>2</v>
       </c>
       <c r="L480" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.3/R2</v>
       </c>
       <c r="M480" s="13" t="s">
@@ -14931,7 +14931,7 @@
         <v>4</v>
       </c>
       <c r="L481" s="13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>C34/G1/G1.4</v>
       </c>
       <c r="M481" s="13" t="s">
@@ -14958,7 +14958,7 @@
         <v>1</v>
       </c>
       <c r="L482" s="13" t="str">
-        <f t="shared" ref="L482:L550" si="13">CONCATENATE(IF(A482="","",CONCATENATE("C", A482)),IF(B482="","",CONCATENATE("/G",B482)),IF(C482="","",CONCATENATE("/R",C482)), IF(D482="","",CONCATENATE("/G",B482,".",D482)), IF(E482="","",CONCATENATE("/R",E482)), IF(F482="","",CONCATENATE("/G",B482,".",D482,".",F482)), IF(G482="","",CONCATENATE("/R",G482)), IF(H482="","",CONCATENATE("/G",B482,".",D482,".",F482,".",H482)), IF(I482="","",CONCATENATE("/R",I482)),IF(J482="","",CONCATENATE("/G",B482,".",D482,".",F482,".",H482, ".",J482)), IF(K482="","",CONCATENATE("/R",K482)))</f>
+        <f t="shared" ref="L482:L550" si="14">CONCATENATE(IF(A482="","",CONCATENATE("C", A482)),IF(B482="","",CONCATENATE("/G",B482)),IF(C482="","",CONCATENATE("/R",C482)), IF(D482="","",CONCATENATE("/G",B482,".",D482)), IF(E482="","",CONCATENATE("/R",E482)), IF(F482="","",CONCATENATE("/G",B482,".",D482,".",F482)), IF(G482="","",CONCATENATE("/R",G482)), IF(H482="","",CONCATENATE("/G",B482,".",D482,".",F482,".",H482)), IF(I482="","",CONCATENATE("/R",I482)),IF(J482="","",CONCATENATE("/G",B482,".",D482,".",F482,".",H482, ".",J482)), IF(K482="","",CONCATENATE("/R",K482)))</f>
         <v>C34/G1/G1.4/R1</v>
       </c>
       <c r="M482" s="13" t="s">
@@ -14988,7 +14988,7 @@
         <v>2</v>
       </c>
       <c r="L483" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G1/G1.4/R2</v>
       </c>
       <c r="M483" s="13" t="s">
@@ -15015,7 +15015,7 @@
         <v>5</v>
       </c>
       <c r="L484" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G1/G1.5</v>
       </c>
       <c r="M484" s="13" t="s">
@@ -15042,7 +15042,7 @@
         <v>1</v>
       </c>
       <c r="L485" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G1/G1.5/R1</v>
       </c>
       <c r="M485" s="13" t="s">
@@ -15072,7 +15072,7 @@
         <v>2</v>
       </c>
       <c r="L486" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G1/G1.5/R2</v>
       </c>
       <c r="M486" s="13" t="s">
@@ -15096,7 +15096,7 @@
         <v>2</v>
       </c>
       <c r="L487" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2</v>
       </c>
       <c r="M487" t="s">
@@ -15117,7 +15117,7 @@
         <v>1</v>
       </c>
       <c r="L488" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2/R1</v>
       </c>
       <c r="M488" t="s">
@@ -15141,7 +15141,7 @@
         <v>1</v>
       </c>
       <c r="L489" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2/G2.1</v>
       </c>
       <c r="M489" t="s">
@@ -15168,7 +15168,7 @@
         <v>1</v>
       </c>
       <c r="L490" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2/G2.1/R1</v>
       </c>
       <c r="M490" t="s">
@@ -15195,7 +15195,7 @@
         <v>2</v>
       </c>
       <c r="L491" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2/G2.1/R2</v>
       </c>
       <c r="M491" t="s">
@@ -15222,7 +15222,7 @@
         <v>3</v>
       </c>
       <c r="L492" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C34/G2/G2.1/R3</v>
       </c>
       <c r="M492" s="6" t="s">
@@ -15240,7 +15240,7 @@
         <v>35</v>
       </c>
       <c r="L493" s="8" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35</v>
       </c>
       <c r="M493" s="8" t="s">
@@ -15262,7 +15262,7 @@
         <v>1</v>
       </c>
       <c r="L494" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G1</v>
       </c>
       <c r="M494" t="s">
@@ -15283,7 +15283,7 @@
         <v>1</v>
       </c>
       <c r="L495" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G1/R1</v>
       </c>
       <c r="M495" t="s">
@@ -15304,7 +15304,7 @@
         <v>2</v>
       </c>
       <c r="L496" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2</v>
       </c>
       <c r="M496" t="s">
@@ -15325,7 +15325,7 @@
         <v>1</v>
       </c>
       <c r="L497" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2/R1</v>
       </c>
       <c r="M497" t="s">
@@ -15349,7 +15349,7 @@
         <v>1</v>
       </c>
       <c r="L498" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2/G2.1</v>
       </c>
       <c r="M498" t="s">
@@ -15376,7 +15376,7 @@
         <v>1</v>
       </c>
       <c r="L499" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2/G2.1/R1</v>
       </c>
       <c r="M499" t="s">
@@ -15403,7 +15403,7 @@
         <v>2</v>
       </c>
       <c r="L500" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2/G2.1/R2</v>
       </c>
       <c r="M500" t="s">
@@ -15430,7 +15430,7 @@
         <v>3</v>
       </c>
       <c r="L501" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C35/G2/G2.1/R3</v>
       </c>
       <c r="M501" s="6" t="s">
@@ -15448,7 +15448,7 @@
         <v>36</v>
       </c>
       <c r="L502" s="8" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36</v>
       </c>
       <c r="M502" s="8" t="s">
@@ -15470,7 +15470,7 @@
         <v>1</v>
       </c>
       <c r="L503" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G1</v>
       </c>
       <c r="M503" t="s">
@@ -15491,7 +15491,7 @@
         <v>1</v>
       </c>
       <c r="L504" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G1/R1</v>
       </c>
       <c r="M504" t="s">
@@ -15512,7 +15512,7 @@
         <v>2</v>
       </c>
       <c r="L505" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2</v>
       </c>
       <c r="M505" t="s">
@@ -15533,7 +15533,7 @@
         <v>1</v>
       </c>
       <c r="L506" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2/R1</v>
       </c>
       <c r="M506" t="s">
@@ -15557,7 +15557,7 @@
         <v>1</v>
       </c>
       <c r="L507" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2/G2.1</v>
       </c>
       <c r="M507" t="s">
@@ -15584,7 +15584,7 @@
         <v>1</v>
       </c>
       <c r="L508" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2/G2.1/R1</v>
       </c>
       <c r="M508" t="s">
@@ -15611,7 +15611,7 @@
         <v>2</v>
       </c>
       <c r="L509" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2/G2.1/R2</v>
       </c>
       <c r="M509" t="s">
@@ -15638,7 +15638,7 @@
         <v>3</v>
       </c>
       <c r="L510" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C36/G2/G2.1/R3</v>
       </c>
       <c r="M510" s="6" t="s">
@@ -15666,7 +15666,7 @@
       <c r="J511" s="4"/>
       <c r="K511" s="4"/>
       <c r="L511" s="4" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37</v>
       </c>
       <c r="M511" s="4" t="s">
@@ -15689,7 +15689,7 @@
         <v>1</v>
       </c>
       <c r="L512" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1</v>
       </c>
       <c r="M512" t="s">
@@ -15713,7 +15713,7 @@
         <v>1</v>
       </c>
       <c r="L513" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1/R1</v>
       </c>
       <c r="M513" t="s">
@@ -15737,7 +15737,7 @@
         <v>2</v>
       </c>
       <c r="L514" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1/R2</v>
       </c>
       <c r="M514" t="s">
@@ -15761,7 +15761,7 @@
         <v>3</v>
       </c>
       <c r="L515" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1/R3</v>
       </c>
       <c r="M515" t="s">
@@ -15788,7 +15788,7 @@
         <v>4</v>
       </c>
       <c r="L516" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1/R4</v>
       </c>
       <c r="M516" s="6" t="s">
@@ -15815,7 +15815,7 @@
         <v>5</v>
       </c>
       <c r="L517" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G1/R5</v>
       </c>
       <c r="M517" t="s">
@@ -15836,7 +15836,7 @@
         <v>2</v>
       </c>
       <c r="L518" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2</v>
       </c>
       <c r="M518" s="13" t="s">
@@ -15860,7 +15860,7 @@
         <v>1</v>
       </c>
       <c r="L519" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/R1</v>
       </c>
       <c r="M519" s="13" t="s">
@@ -15887,7 +15887,7 @@
         <v>2</v>
       </c>
       <c r="L520" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/R2</v>
       </c>
       <c r="M520" s="13" t="s">
@@ -15914,7 +15914,7 @@
         <v>3</v>
       </c>
       <c r="L521" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/R3</v>
       </c>
       <c r="M521" s="13" t="s">
@@ -15941,7 +15941,7 @@
         <v>4</v>
       </c>
       <c r="L522" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/R4</v>
       </c>
       <c r="M522" s="13" t="s">
@@ -15965,7 +15965,7 @@
         <v>3</v>
       </c>
       <c r="L523" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G3</v>
       </c>
       <c r="M523" s="13" t="s">
@@ -15989,7 +15989,7 @@
         <v>1</v>
       </c>
       <c r="L524" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G3/R1</v>
       </c>
       <c r="M524" s="13" t="s">
@@ -16016,7 +16016,7 @@
         <v>2</v>
       </c>
       <c r="L525" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G3/R2</v>
       </c>
       <c r="M525" s="13" t="s">
@@ -16043,7 +16043,7 @@
         <v>3</v>
       </c>
       <c r="L526" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G3/R3</v>
       </c>
       <c r="M526" s="13" t="s">
@@ -16070,7 +16070,7 @@
         <v>4</v>
       </c>
       <c r="L527" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G3/R4</v>
       </c>
       <c r="M527" s="13" t="s">
@@ -16094,7 +16094,7 @@
         <v>4</v>
       </c>
       <c r="L528" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G4</v>
       </c>
       <c r="M528" s="13" t="s">
@@ -16118,7 +16118,7 @@
         <v>1</v>
       </c>
       <c r="L529" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G4/R1</v>
       </c>
       <c r="M529" s="13" t="s">
@@ -16145,7 +16145,7 @@
         <v>2</v>
       </c>
       <c r="L530" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G4/R2</v>
       </c>
       <c r="M530" s="13" t="s">
@@ -16172,7 +16172,7 @@
         <v>3</v>
       </c>
       <c r="L531" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G4/R3</v>
       </c>
       <c r="M531" s="13" t="s">
@@ -16199,7 +16199,7 @@
         <v>4</v>
       </c>
       <c r="L532" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G4/R4</v>
       </c>
       <c r="M532" s="13" t="s">
@@ -16223,7 +16223,7 @@
         <v>5</v>
       </c>
       <c r="L533" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G5</v>
       </c>
       <c r="M533" s="13" t="s">
@@ -16247,7 +16247,7 @@
         <v>1</v>
       </c>
       <c r="L534" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G5/R1</v>
       </c>
       <c r="M534" s="13" t="s">
@@ -16274,7 +16274,7 @@
         <v>2</v>
       </c>
       <c r="L535" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G5/R2</v>
       </c>
       <c r="M535" s="13" t="s">
@@ -16301,7 +16301,7 @@
         <v>3</v>
       </c>
       <c r="L536" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G5/R3</v>
       </c>
       <c r="M536" s="13" t="s">
@@ -16328,7 +16328,7 @@
         <v>4</v>
       </c>
       <c r="L537" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G5/R4</v>
       </c>
       <c r="M537" s="13" t="s">
@@ -16352,7 +16352,7 @@
         <v>2</v>
       </c>
       <c r="L538" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2</v>
       </c>
       <c r="M538" t="s">
@@ -16373,7 +16373,7 @@
         <v>1</v>
       </c>
       <c r="L539" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/R1</v>
       </c>
       <c r="M539" t="s">
@@ -16397,7 +16397,7 @@
         <v>1</v>
       </c>
       <c r="L540" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/G2.1</v>
       </c>
       <c r="M540" t="s">
@@ -16424,7 +16424,7 @@
         <v>1</v>
       </c>
       <c r="L541" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/G2.1/R1</v>
       </c>
       <c r="M541" t="s">
@@ -16451,7 +16451,7 @@
         <v>2</v>
       </c>
       <c r="L542" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/G2.1/R2</v>
       </c>
       <c r="M542" t="s">
@@ -16478,7 +16478,7 @@
         <v>3</v>
       </c>
       <c r="L543" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C37/G2/G2.1/R3</v>
       </c>
       <c r="M543" s="6" t="s">
@@ -16496,7 +16496,7 @@
         <v>38</v>
       </c>
       <c r="L544" s="8" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38</v>
       </c>
       <c r="M544" s="8" t="s">
@@ -16518,7 +16518,7 @@
         <v>1</v>
       </c>
       <c r="L545" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1</v>
       </c>
       <c r="M545" t="s">
@@ -16542,7 +16542,7 @@
         <v>1</v>
       </c>
       <c r="L546" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1/R1</v>
       </c>
       <c r="M546" t="s">
@@ -16566,7 +16566,7 @@
         <v>2</v>
       </c>
       <c r="L547" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1/R2</v>
       </c>
       <c r="M547" t="s">
@@ -16590,7 +16590,7 @@
         <v>3</v>
       </c>
       <c r="L548" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1/R3</v>
       </c>
       <c r="M548" t="s">
@@ -16617,7 +16617,7 @@
         <v>4</v>
       </c>
       <c r="L549" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1/R4</v>
       </c>
       <c r="M549" t="s">
@@ -16644,7 +16644,7 @@
         <v>5</v>
       </c>
       <c r="L550" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>C38/G1/R5</v>
       </c>
       <c r="M550" t="s">
@@ -16665,7 +16665,7 @@
         <v>2</v>
       </c>
       <c r="L551" s="13" t="str">
-        <f t="shared" ref="L551:L618" si="14">CONCATENATE(IF(A551="","",CONCATENATE("C", A551)),IF(B551="","",CONCATENATE("/G",B551)),IF(C551="","",CONCATENATE("/R",C551)), IF(D551="","",CONCATENATE("/G",B551,".",D551)), IF(E551="","",CONCATENATE("/R",E551)), IF(F551="","",CONCATENATE("/G",B551,".",D551,".",F551)), IF(G551="","",CONCATENATE("/R",G551)), IF(H551="","",CONCATENATE("/G",B551,".",D551,".",F551,".",H551)), IF(I551="","",CONCATENATE("/R",I551)),IF(J551="","",CONCATENATE("/G",B551,".",D551,".",F551,".",H551, ".",J551)), IF(K551="","",CONCATENATE("/R",K551)))</f>
+        <f t="shared" ref="L551:L618" si="15">CONCATENATE(IF(A551="","",CONCATENATE("C", A551)),IF(B551="","",CONCATENATE("/G",B551)),IF(C551="","",CONCATENATE("/R",C551)), IF(D551="","",CONCATENATE("/G",B551,".",D551)), IF(E551="","",CONCATENATE("/R",E551)), IF(F551="","",CONCATENATE("/G",B551,".",D551,".",F551)), IF(G551="","",CONCATENATE("/R",G551)), IF(H551="","",CONCATENATE("/G",B551,".",D551,".",F551,".",H551)), IF(I551="","",CONCATENATE("/R",I551)),IF(J551="","",CONCATENATE("/G",B551,".",D551,".",F551,".",H551, ".",J551)), IF(K551="","",CONCATENATE("/R",K551)))</f>
         <v>C38/G2</v>
       </c>
       <c r="M551" s="13" t="s">
@@ -16689,7 +16689,7 @@
         <v>1</v>
       </c>
       <c r="L552" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/R1</v>
       </c>
       <c r="M552" s="13" t="s">
@@ -16716,7 +16716,7 @@
         <v>2</v>
       </c>
       <c r="L553" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/R2</v>
       </c>
       <c r="M553" s="13" t="s">
@@ -16743,7 +16743,7 @@
         <v>3</v>
       </c>
       <c r="L554" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/R3</v>
       </c>
       <c r="M554" s="13" t="s">
@@ -16770,7 +16770,7 @@
         <v>4</v>
       </c>
       <c r="L555" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/R4</v>
       </c>
       <c r="M555" s="13" t="s">
@@ -16794,7 +16794,7 @@
         <v>3</v>
       </c>
       <c r="L556" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G3</v>
       </c>
       <c r="M556" s="13" t="s">
@@ -16818,7 +16818,7 @@
         <v>1</v>
       </c>
       <c r="L557" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G3/R1</v>
       </c>
       <c r="M557" s="13" t="s">
@@ -16845,7 +16845,7 @@
         <v>2</v>
       </c>
       <c r="L558" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G3/R2</v>
       </c>
       <c r="M558" s="13" t="s">
@@ -16872,7 +16872,7 @@
         <v>3</v>
       </c>
       <c r="L559" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G3/R3</v>
       </c>
       <c r="M559" s="13" t="s">
@@ -16899,7 +16899,7 @@
         <v>4</v>
       </c>
       <c r="L560" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G3/R4</v>
       </c>
       <c r="M560" s="13" t="s">
@@ -16923,7 +16923,7 @@
         <v>4</v>
       </c>
       <c r="L561" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G4</v>
       </c>
       <c r="M561" s="13" t="s">
@@ -16947,7 +16947,7 @@
         <v>1</v>
       </c>
       <c r="L562" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G4/R1</v>
       </c>
       <c r="M562" s="13" t="s">
@@ -16974,7 +16974,7 @@
         <v>2</v>
       </c>
       <c r="L563" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G4/R2</v>
       </c>
       <c r="M563" s="13" t="s">
@@ -17001,7 +17001,7 @@
         <v>3</v>
       </c>
       <c r="L564" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G4/R3</v>
       </c>
       <c r="M564" s="13" t="s">
@@ -17028,7 +17028,7 @@
         <v>4</v>
       </c>
       <c r="L565" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G4/R4</v>
       </c>
       <c r="M565" s="13" t="s">
@@ -17052,7 +17052,7 @@
         <v>5</v>
       </c>
       <c r="L566" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G5</v>
       </c>
       <c r="M566" s="13" t="s">
@@ -17076,7 +17076,7 @@
         <v>1</v>
       </c>
       <c r="L567" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G5/R1</v>
       </c>
       <c r="M567" s="13" t="s">
@@ -17103,7 +17103,7 @@
         <v>2</v>
       </c>
       <c r="L568" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G5/R2</v>
       </c>
       <c r="M568" s="13" t="s">
@@ -17130,7 +17130,7 @@
         <v>3</v>
       </c>
       <c r="L569" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G5/R3</v>
       </c>
       <c r="M569" s="13" t="s">
@@ -17157,7 +17157,7 @@
         <v>4</v>
       </c>
       <c r="L570" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G5/R4</v>
       </c>
       <c r="M570" s="13" t="s">
@@ -17181,7 +17181,7 @@
         <v>2</v>
       </c>
       <c r="L571" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2</v>
       </c>
       <c r="M571" t="s">
@@ -17202,7 +17202,7 @@
         <v>1</v>
       </c>
       <c r="L572" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/R1</v>
       </c>
       <c r="M572" t="s">
@@ -17226,7 +17226,7 @@
         <v>1</v>
       </c>
       <c r="L573" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/G2.1</v>
       </c>
       <c r="M573" t="s">
@@ -17253,7 +17253,7 @@
         <v>1</v>
       </c>
       <c r="L574" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/G2.1/R1</v>
       </c>
       <c r="M574" t="s">
@@ -17280,7 +17280,7 @@
         <v>2</v>
       </c>
       <c r="L575" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/G2.1/R2</v>
       </c>
       <c r="M575" t="s">
@@ -17307,7 +17307,7 @@
         <v>3</v>
       </c>
       <c r="L576" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C38/G2/G2.1/R3</v>
       </c>
       <c r="M576" s="6" t="s">
@@ -17325,7 +17325,7 @@
         <v>39</v>
       </c>
       <c r="L577" s="8" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39</v>
       </c>
       <c r="M577" s="8" t="s">
@@ -17347,7 +17347,7 @@
         <v>1</v>
       </c>
       <c r="L578" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G1</v>
       </c>
       <c r="M578" t="s">
@@ -17371,7 +17371,7 @@
         <v>1</v>
       </c>
       <c r="L579" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G1/R1</v>
       </c>
       <c r="M579" t="s">
@@ -17395,7 +17395,7 @@
         <v>2</v>
       </c>
       <c r="L580" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G1/R2</v>
       </c>
       <c r="M580" t="s">
@@ -17419,7 +17419,7 @@
         <v>3</v>
       </c>
       <c r="L581" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G1/R3</v>
       </c>
       <c r="M581" t="s">
@@ -17473,7 +17473,7 @@
         <v>5</v>
       </c>
       <c r="L583" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G1/R5</v>
       </c>
       <c r="M583" t="s">
@@ -17494,7 +17494,7 @@
         <v>2</v>
       </c>
       <c r="L584" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2</v>
       </c>
       <c r="M584" s="13" t="s">
@@ -17518,7 +17518,7 @@
         <v>1</v>
       </c>
       <c r="L585" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/R1</v>
       </c>
       <c r="M585" s="13" t="s">
@@ -17545,7 +17545,7 @@
         <v>2</v>
       </c>
       <c r="L586" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/R2</v>
       </c>
       <c r="M586" s="13" t="s">
@@ -17572,7 +17572,7 @@
         <v>3</v>
       </c>
       <c r="L587" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/R3</v>
       </c>
       <c r="M587" s="13" t="s">
@@ -17599,7 +17599,7 @@
         <v>4</v>
       </c>
       <c r="L588" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/R4</v>
       </c>
       <c r="M588" s="13" t="s">
@@ -17623,7 +17623,7 @@
         <v>3</v>
       </c>
       <c r="L589" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G3</v>
       </c>
       <c r="M589" s="13" t="s">
@@ -17647,7 +17647,7 @@
         <v>1</v>
       </c>
       <c r="L590" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G3/R1</v>
       </c>
       <c r="M590" s="13" t="s">
@@ -17674,7 +17674,7 @@
         <v>2</v>
       </c>
       <c r="L591" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G3/R2</v>
       </c>
       <c r="M591" s="13" t="s">
@@ -17701,7 +17701,7 @@
         <v>3</v>
       </c>
       <c r="L592" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G3/R3</v>
       </c>
       <c r="M592" s="13" t="s">
@@ -17728,7 +17728,7 @@
         <v>4</v>
       </c>
       <c r="L593" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G3/R4</v>
       </c>
       <c r="M593" s="13" t="s">
@@ -17752,7 +17752,7 @@
         <v>4</v>
       </c>
       <c r="L594" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G4</v>
       </c>
       <c r="M594" s="13" t="s">
@@ -17776,7 +17776,7 @@
         <v>1</v>
       </c>
       <c r="L595" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G4/R1</v>
       </c>
       <c r="M595" s="13" t="s">
@@ -17803,7 +17803,7 @@
         <v>2</v>
       </c>
       <c r="L596" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G4/R2</v>
       </c>
       <c r="M596" s="13" t="s">
@@ -17830,7 +17830,7 @@
         <v>3</v>
       </c>
       <c r="L597" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G4/R3</v>
       </c>
       <c r="M597" s="13" t="s">
@@ -17857,7 +17857,7 @@
         <v>4</v>
       </c>
       <c r="L598" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G4/R4</v>
       </c>
       <c r="M598" s="13" t="s">
@@ -17881,7 +17881,7 @@
         <v>5</v>
       </c>
       <c r="L599" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G5</v>
       </c>
       <c r="M599" s="13" t="s">
@@ -17905,7 +17905,7 @@
         <v>1</v>
       </c>
       <c r="L600" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G5/R1</v>
       </c>
       <c r="M600" s="13" t="s">
@@ -17932,7 +17932,7 @@
         <v>2</v>
       </c>
       <c r="L601" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G5/R2</v>
       </c>
       <c r="M601" s="13" t="s">
@@ -17959,7 +17959,7 @@
         <v>3</v>
       </c>
       <c r="L602" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G5/R3</v>
       </c>
       <c r="M602" s="13" t="s">
@@ -17986,7 +17986,7 @@
         <v>4</v>
       </c>
       <c r="L603" s="13" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G5/R4</v>
       </c>
       <c r="M603" s="13" t="s">
@@ -18010,7 +18010,7 @@
         <v>2</v>
       </c>
       <c r="L604" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2</v>
       </c>
       <c r="M604" t="s">
@@ -18031,7 +18031,7 @@
         <v>1</v>
       </c>
       <c r="L605" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/R1</v>
       </c>
       <c r="M605" t="s">
@@ -18055,7 +18055,7 @@
         <v>1</v>
       </c>
       <c r="L606" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/G2.1</v>
       </c>
       <c r="M606" t="s">
@@ -18082,7 +18082,7 @@
         <v>1</v>
       </c>
       <c r="L607" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/G2.1/R1</v>
       </c>
       <c r="M607" t="s">
@@ -18109,7 +18109,7 @@
         <v>2</v>
       </c>
       <c r="L608" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/G2.1/R2</v>
       </c>
       <c r="M608" t="s">
@@ -18136,7 +18136,7 @@
         <v>3</v>
       </c>
       <c r="L609" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C39/G2/G2.1/R3</v>
       </c>
       <c r="M609" s="6" t="s">
@@ -18154,7 +18154,7 @@
         <v>40</v>
       </c>
       <c r="L610" s="8" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40</v>
       </c>
       <c r="M610" s="8" t="s">
@@ -18176,7 +18176,7 @@
         <v>1</v>
       </c>
       <c r="L611" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G1</v>
       </c>
       <c r="M611" t="s">
@@ -18197,7 +18197,7 @@
         <v>1</v>
       </c>
       <c r="L612" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G1/R1</v>
       </c>
       <c r="M612" t="s">
@@ -18218,7 +18218,7 @@
         <v>2</v>
       </c>
       <c r="L613" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2</v>
       </c>
       <c r="M613" t="s">
@@ -18239,7 +18239,7 @@
         <v>1</v>
       </c>
       <c r="L614" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2/R1</v>
       </c>
       <c r="M614" t="s">
@@ -18263,7 +18263,7 @@
         <v>1</v>
       </c>
       <c r="L615" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2/G2.1</v>
       </c>
       <c r="M615" t="s">
@@ -18290,7 +18290,7 @@
         <v>1</v>
       </c>
       <c r="L616" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2/G2.1/R1</v>
       </c>
       <c r="M616" t="s">
@@ -18317,7 +18317,7 @@
         <v>2</v>
       </c>
       <c r="L617" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2/G2.1/R2</v>
       </c>
       <c r="M617" t="s">
@@ -18344,7 +18344,7 @@
         <v>3</v>
       </c>
       <c r="L618" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>C40/G2/G2.1/R3</v>
       </c>
       <c r="M618" s="6" t="s">
@@ -18362,7 +18362,7 @@
         <v>41</v>
       </c>
       <c r="L619" s="8" t="str">
-        <f t="shared" ref="L619:L696" si="15">CONCATENATE(IF(A619="","",CONCATENATE("C", A619)),IF(B619="","",CONCATENATE("/G",B619)),IF(C619="","",CONCATENATE("/R",C619)), IF(D619="","",CONCATENATE("/G",B619,".",D619)), IF(E619="","",CONCATENATE("/R",E619)), IF(F619="","",CONCATENATE("/G",B619,".",D619,".",F619)), IF(G619="","",CONCATENATE("/R",G619)), IF(H619="","",CONCATENATE("/G",B619,".",D619,".",F619,".",H619)), IF(I619="","",CONCATENATE("/R",I619)),IF(J619="","",CONCATENATE("/G",B619,".",D619,".",F619,".",H619, ".",J619)), IF(K619="","",CONCATENATE("/R",K619)))</f>
+        <f t="shared" ref="L619:L696" si="16">CONCATENATE(IF(A619="","",CONCATENATE("C", A619)),IF(B619="","",CONCATENATE("/G",B619)),IF(C619="","",CONCATENATE("/R",C619)), IF(D619="","",CONCATENATE("/G",B619,".",D619)), IF(E619="","",CONCATENATE("/R",E619)), IF(F619="","",CONCATENATE("/G",B619,".",D619,".",F619)), IF(G619="","",CONCATENATE("/R",G619)), IF(H619="","",CONCATENATE("/G",B619,".",D619,".",F619,".",H619)), IF(I619="","",CONCATENATE("/R",I619)),IF(J619="","",CONCATENATE("/G",B619,".",D619,".",F619,".",H619, ".",J619)), IF(K619="","",CONCATENATE("/R",K619)))</f>
         <v>C41</v>
       </c>
       <c r="M619" s="8" t="s">
@@ -18384,7 +18384,7 @@
         <v>1</v>
       </c>
       <c r="L620" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G1</v>
       </c>
       <c r="M620" t="s">
@@ -18405,7 +18405,7 @@
         <v>1</v>
       </c>
       <c r="L621" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G1/R1</v>
       </c>
       <c r="M621" t="s">
@@ -18426,7 +18426,7 @@
         <v>2</v>
       </c>
       <c r="L622" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2</v>
       </c>
       <c r="M622" t="s">
@@ -18447,7 +18447,7 @@
         <v>1</v>
       </c>
       <c r="L623" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2/R1</v>
       </c>
       <c r="M623" t="s">
@@ -18471,7 +18471,7 @@
         <v>1</v>
       </c>
       <c r="L624" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2/G2.1</v>
       </c>
       <c r="M624" t="s">
@@ -18498,7 +18498,7 @@
         <v>1</v>
       </c>
       <c r="L625" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2/G2.1/R1</v>
       </c>
       <c r="M625" t="s">
@@ -18525,7 +18525,7 @@
         <v>2</v>
       </c>
       <c r="L626" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2/G2.1/R2</v>
       </c>
       <c r="M626" t="s">
@@ -18552,7 +18552,7 @@
         <v>3</v>
       </c>
       <c r="L627" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C41/G2/G2.1/R3</v>
       </c>
       <c r="M627" s="6" t="s">
@@ -18570,7 +18570,7 @@
         <v>42</v>
       </c>
       <c r="L628" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42</v>
       </c>
       <c r="M628" s="8" t="s">
@@ -18592,7 +18592,7 @@
         <v>1</v>
       </c>
       <c r="L629" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G1</v>
       </c>
       <c r="M629" t="s">
@@ -18613,7 +18613,7 @@
         <v>1</v>
       </c>
       <c r="L630" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G1/R1</v>
       </c>
       <c r="M630" t="s">
@@ -18634,7 +18634,7 @@
         <v>2</v>
       </c>
       <c r="L631" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2</v>
       </c>
       <c r="M631" t="s">
@@ -18655,7 +18655,7 @@
         <v>1</v>
       </c>
       <c r="L632" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2/R1</v>
       </c>
       <c r="M632" t="s">
@@ -18679,7 +18679,7 @@
         <v>1</v>
       </c>
       <c r="L633" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2/G2.1</v>
       </c>
       <c r="M633" t="s">
@@ -18706,7 +18706,7 @@
         <v>1</v>
       </c>
       <c r="L634" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2/G2.1/R1</v>
       </c>
       <c r="M634" t="s">
@@ -18733,7 +18733,7 @@
         <v>2</v>
       </c>
       <c r="L635" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2/G2.1/R2</v>
       </c>
       <c r="M635" t="s">
@@ -18760,7 +18760,7 @@
         <v>3</v>
       </c>
       <c r="L636" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C42/G2/G2.1/R3</v>
       </c>
       <c r="M636" s="6" t="s">
@@ -18778,7 +18778,7 @@
         <v>43</v>
       </c>
       <c r="L637" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43</v>
       </c>
       <c r="M637" s="8" t="s">
@@ -18800,7 +18800,7 @@
         <v>1</v>
       </c>
       <c r="L638" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G1</v>
       </c>
       <c r="M638" t="s">
@@ -18821,7 +18821,7 @@
         <v>1</v>
       </c>
       <c r="L639" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G1/R1</v>
       </c>
       <c r="M639" t="s">
@@ -18842,7 +18842,7 @@
         <v>2</v>
       </c>
       <c r="L640" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2</v>
       </c>
       <c r="M640" t="s">
@@ -18863,7 +18863,7 @@
         <v>1</v>
       </c>
       <c r="L641" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2/R1</v>
       </c>
       <c r="M641" t="s">
@@ -18887,7 +18887,7 @@
         <v>1</v>
       </c>
       <c r="L642" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2/G2.1</v>
       </c>
       <c r="M642" t="s">
@@ -18914,7 +18914,7 @@
         <v>1</v>
       </c>
       <c r="L643" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2/G2.1/R1</v>
       </c>
       <c r="M643" t="s">
@@ -18941,7 +18941,7 @@
         <v>2</v>
       </c>
       <c r="L644" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2/G2.1/R2</v>
       </c>
       <c r="M644" t="s">
@@ -18968,7 +18968,7 @@
         <v>3</v>
       </c>
       <c r="L645" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C43/G2/G2.1/R3</v>
       </c>
       <c r="M645" s="6" t="s">
@@ -18986,7 +18986,7 @@
         <v>44</v>
       </c>
       <c r="L646" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44</v>
       </c>
       <c r="M646" s="8" t="s">
@@ -19008,7 +19008,7 @@
         <v>1</v>
       </c>
       <c r="L647" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G1</v>
       </c>
       <c r="M647" t="s">
@@ -19029,7 +19029,7 @@
         <v>1</v>
       </c>
       <c r="L648" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G1/R1</v>
       </c>
       <c r="M648" t="s">
@@ -19050,7 +19050,7 @@
         <v>2</v>
       </c>
       <c r="L649" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2</v>
       </c>
       <c r="M649" t="s">
@@ -19071,7 +19071,7 @@
         <v>1</v>
       </c>
       <c r="L650" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2/R1</v>
       </c>
       <c r="M650" t="s">
@@ -19095,7 +19095,7 @@
         <v>1</v>
       </c>
       <c r="L651" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2/G2.1</v>
       </c>
       <c r="M651" t="s">
@@ -19122,7 +19122,7 @@
         <v>1</v>
       </c>
       <c r="L652" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2/G2.1/R1</v>
       </c>
       <c r="M652" t="s">
@@ -19149,7 +19149,7 @@
         <v>2</v>
       </c>
       <c r="L653" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2/G2.1/R2</v>
       </c>
       <c r="M653" t="s">
@@ -19176,7 +19176,7 @@
         <v>3</v>
       </c>
       <c r="L654" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C44/G2/G2.1/R3</v>
       </c>
       <c r="M654" s="6" t="s">
@@ -19194,7 +19194,7 @@
         <v>45</v>
       </c>
       <c r="L655" s="8" t="str">
-        <f>CONCATENATE(IF(A655="","",CONCATENATE("C", A655)),IF(B655="","",CONCATENATE("/G",B655)),IF(C655="","",CONCATENATE("/R",C655)), IF(D655="","",CONCATENATE("/G",B655,".",D655)), IF(E655="","",CONCATENATE("/R",E655)), IF(F655="","",CONCATENATE("/G",B655,".",D655,".",F655)), IF(G655="","",CONCATENATE("/R",G655)), IF(H655="","",CONCATENATE("/G",B655,".",D655,".",F655,".",H655)), IF(I655="","",CONCATENATE("/R",I655)),IF(J655="","",CONCATENATE("/G",B655,".",D655,".",F655,".",H655, ".",J655)), IF(K655="","",CONCATENATE("/R",K655)))</f>
+        <f t="shared" ref="L655:L681" si="17">CONCATENATE(IF(A655="","",CONCATENATE("C", A655)),IF(B655="","",CONCATENATE("/G",B655)),IF(C655="","",CONCATENATE("/R",C655)), IF(D655="","",CONCATENATE("/G",B655,".",D655)), IF(E655="","",CONCATENATE("/R",E655)), IF(F655="","",CONCATENATE("/G",B655,".",D655,".",F655)), IF(G655="","",CONCATENATE("/R",G655)), IF(H655="","",CONCATENATE("/G",B655,".",D655,".",F655,".",H655)), IF(I655="","",CONCATENATE("/R",I655)),IF(J655="","",CONCATENATE("/G",B655,".",D655,".",F655,".",H655, ".",J655)), IF(K655="","",CONCATENATE("/R",K655)))</f>
         <v>C45</v>
       </c>
       <c r="M655" s="8" t="s">
@@ -19216,7 +19216,7 @@
         <v>1</v>
       </c>
       <c r="L656" t="str">
-        <f>CONCATENATE(IF(A656="","",CONCATENATE("C", A656)),IF(B656="","",CONCATENATE("/G",B656)),IF(C656="","",CONCATENATE("/R",C656)), IF(D656="","",CONCATENATE("/G",B656,".",D656)), IF(E656="","",CONCATENATE("/R",E656)), IF(F656="","",CONCATENATE("/G",B656,".",D656,".",F656)), IF(G656="","",CONCATENATE("/R",G656)), IF(H656="","",CONCATENATE("/G",B656,".",D656,".",F656,".",H656)), IF(I656="","",CONCATENATE("/R",I656)),IF(J656="","",CONCATENATE("/G",B656,".",D656,".",F656,".",H656, ".",J656)), IF(K656="","",CONCATENATE("/R",K656)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G1</v>
       </c>
       <c r="M656" t="s">
@@ -19237,7 +19237,7 @@
         <v>1</v>
       </c>
       <c r="L657" t="str">
-        <f>CONCATENATE(IF(A657="","",CONCATENATE("C", A657)),IF(B657="","",CONCATENATE("/G",B657)),IF(C657="","",CONCATENATE("/R",C657)), IF(D657="","",CONCATENATE("/G",B657,".",D657)), IF(E657="","",CONCATENATE("/R",E657)), IF(F657="","",CONCATENATE("/G",B657,".",D657,".",F657)), IF(G657="","",CONCATENATE("/R",G657)), IF(H657="","",CONCATENATE("/G",B657,".",D657,".",F657,".",H657)), IF(I657="","",CONCATENATE("/R",I657)),IF(J657="","",CONCATENATE("/G",B657,".",D657,".",F657,".",H657, ".",J657)), IF(K657="","",CONCATENATE("/R",K657)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G1/R1</v>
       </c>
       <c r="M657" t="s">
@@ -19258,7 +19258,7 @@
         <v>2</v>
       </c>
       <c r="L658" t="str">
-        <f>CONCATENATE(IF(A658="","",CONCATENATE("C", A658)),IF(B658="","",CONCATENATE("/G",B658)),IF(C658="","",CONCATENATE("/R",C658)), IF(D658="","",CONCATENATE("/G",B658,".",D658)), IF(E658="","",CONCATENATE("/R",E658)), IF(F658="","",CONCATENATE("/G",B658,".",D658,".",F658)), IF(G658="","",CONCATENATE("/R",G658)), IF(H658="","",CONCATENATE("/G",B658,".",D658,".",F658,".",H658)), IF(I658="","",CONCATENATE("/R",I658)),IF(J658="","",CONCATENATE("/G",B658,".",D658,".",F658,".",H658, ".",J658)), IF(K658="","",CONCATENATE("/R",K658)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2</v>
       </c>
       <c r="M658" t="s">
@@ -19279,7 +19279,7 @@
         <v>1</v>
       </c>
       <c r="L659" t="str">
-        <f>CONCATENATE(IF(A659="","",CONCATENATE("C", A659)),IF(B659="","",CONCATENATE("/G",B659)),IF(C659="","",CONCATENATE("/R",C659)), IF(D659="","",CONCATENATE("/G",B659,".",D659)), IF(E659="","",CONCATENATE("/R",E659)), IF(F659="","",CONCATENATE("/G",B659,".",D659,".",F659)), IF(G659="","",CONCATENATE("/R",G659)), IF(H659="","",CONCATENATE("/G",B659,".",D659,".",F659,".",H659)), IF(I659="","",CONCATENATE("/R",I659)),IF(J659="","",CONCATENATE("/G",B659,".",D659,".",F659,".",H659, ".",J659)), IF(K659="","",CONCATENATE("/R",K659)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2/R1</v>
       </c>
       <c r="M659" t="s">
@@ -19303,7 +19303,7 @@
         <v>1</v>
       </c>
       <c r="L660" t="str">
-        <f>CONCATENATE(IF(A660="","",CONCATENATE("C", A660)),IF(B660="","",CONCATENATE("/G",B660)),IF(C660="","",CONCATENATE("/R",C660)), IF(D660="","",CONCATENATE("/G",B660,".",D660)), IF(E660="","",CONCATENATE("/R",E660)), IF(F660="","",CONCATENATE("/G",B660,".",D660,".",F660)), IF(G660="","",CONCATENATE("/R",G660)), IF(H660="","",CONCATENATE("/G",B660,".",D660,".",F660,".",H660)), IF(I660="","",CONCATENATE("/R",I660)),IF(J660="","",CONCATENATE("/G",B660,".",D660,".",F660,".",H660, ".",J660)), IF(K660="","",CONCATENATE("/R",K660)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2/G2.1</v>
       </c>
       <c r="M660" t="s">
@@ -19330,7 +19330,7 @@
         <v>1</v>
       </c>
       <c r="L661" t="str">
-        <f>CONCATENATE(IF(A661="","",CONCATENATE("C", A661)),IF(B661="","",CONCATENATE("/G",B661)),IF(C661="","",CONCATENATE("/R",C661)), IF(D661="","",CONCATENATE("/G",B661,".",D661)), IF(E661="","",CONCATENATE("/R",E661)), IF(F661="","",CONCATENATE("/G",B661,".",D661,".",F661)), IF(G661="","",CONCATENATE("/R",G661)), IF(H661="","",CONCATENATE("/G",B661,".",D661,".",F661,".",H661)), IF(I661="","",CONCATENATE("/R",I661)),IF(J661="","",CONCATENATE("/G",B661,".",D661,".",F661,".",H661, ".",J661)), IF(K661="","",CONCATENATE("/R",K661)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2/G2.1/R1</v>
       </c>
       <c r="M661" t="s">
@@ -19357,7 +19357,7 @@
         <v>2</v>
       </c>
       <c r="L662" t="str">
-        <f>CONCATENATE(IF(A662="","",CONCATENATE("C", A662)),IF(B662="","",CONCATENATE("/G",B662)),IF(C662="","",CONCATENATE("/R",C662)), IF(D662="","",CONCATENATE("/G",B662,".",D662)), IF(E662="","",CONCATENATE("/R",E662)), IF(F662="","",CONCATENATE("/G",B662,".",D662,".",F662)), IF(G662="","",CONCATENATE("/R",G662)), IF(H662="","",CONCATENATE("/G",B662,".",D662,".",F662,".",H662)), IF(I662="","",CONCATENATE("/R",I662)),IF(J662="","",CONCATENATE("/G",B662,".",D662,".",F662,".",H662, ".",J662)), IF(K662="","",CONCATENATE("/R",K662)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2/G2.1/R2</v>
       </c>
       <c r="M662" t="s">
@@ -19384,7 +19384,7 @@
         <v>3</v>
       </c>
       <c r="L663" s="6" t="str">
-        <f>CONCATENATE(IF(A663="","",CONCATENATE("C", A663)),IF(B663="","",CONCATENATE("/G",B663)),IF(C663="","",CONCATENATE("/R",C663)), IF(D663="","",CONCATENATE("/G",B663,".",D663)), IF(E663="","",CONCATENATE("/R",E663)), IF(F663="","",CONCATENATE("/G",B663,".",D663,".",F663)), IF(G663="","",CONCATENATE("/R",G663)), IF(H663="","",CONCATENATE("/G",B663,".",D663,".",F663,".",H663)), IF(I663="","",CONCATENATE("/R",I663)),IF(J663="","",CONCATENATE("/G",B663,".",D663,".",F663,".",H663, ".",J663)), IF(K663="","",CONCATENATE("/R",K663)))</f>
+        <f t="shared" si="17"/>
         <v>C45/G2/G2.1/R3</v>
       </c>
       <c r="M663" s="6" t="s">
@@ -19402,7 +19402,7 @@
         <v>46</v>
       </c>
       <c r="L664" s="8" t="str">
-        <f>CONCATENATE(IF(A664="","",CONCATENATE("C", A664)),IF(B664="","",CONCATENATE("/G",B664)),IF(C664="","",CONCATENATE("/R",C664)), IF(D664="","",CONCATENATE("/G",B664,".",D664)), IF(E664="","",CONCATENATE("/R",E664)), IF(F664="","",CONCATENATE("/G",B664,".",D664,".",F664)), IF(G664="","",CONCATENATE("/R",G664)), IF(H664="","",CONCATENATE("/G",B664,".",D664,".",F664,".",H664)), IF(I664="","",CONCATENATE("/R",I664)),IF(J664="","",CONCATENATE("/G",B664,".",D664,".",F664,".",H664, ".",J664)), IF(K664="","",CONCATENATE("/R",K664)))</f>
+        <f t="shared" si="17"/>
         <v>C46</v>
       </c>
       <c r="M664" s="8" t="s">
@@ -19424,7 +19424,7 @@
         <v>1</v>
       </c>
       <c r="L665" t="str">
-        <f>CONCATENATE(IF(A665="","",CONCATENATE("C", A665)),IF(B665="","",CONCATENATE("/G",B665)),IF(C665="","",CONCATENATE("/R",C665)), IF(D665="","",CONCATENATE("/G",B665,".",D665)), IF(E665="","",CONCATENATE("/R",E665)), IF(F665="","",CONCATENATE("/G",B665,".",D665,".",F665)), IF(G665="","",CONCATENATE("/R",G665)), IF(H665="","",CONCATENATE("/G",B665,".",D665,".",F665,".",H665)), IF(I665="","",CONCATENATE("/R",I665)),IF(J665="","",CONCATENATE("/G",B665,".",D665,".",F665,".",H665, ".",J665)), IF(K665="","",CONCATENATE("/R",K665)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G1</v>
       </c>
       <c r="M665" t="s">
@@ -19445,7 +19445,7 @@
         <v>1</v>
       </c>
       <c r="L666" t="str">
-        <f>CONCATENATE(IF(A666="","",CONCATENATE("C", A666)),IF(B666="","",CONCATENATE("/G",B666)),IF(C666="","",CONCATENATE("/R",C666)), IF(D666="","",CONCATENATE("/G",B666,".",D666)), IF(E666="","",CONCATENATE("/R",E666)), IF(F666="","",CONCATENATE("/G",B666,".",D666,".",F666)), IF(G666="","",CONCATENATE("/R",G666)), IF(H666="","",CONCATENATE("/G",B666,".",D666,".",F666,".",H666)), IF(I666="","",CONCATENATE("/R",I666)),IF(J666="","",CONCATENATE("/G",B666,".",D666,".",F666,".",H666, ".",J666)), IF(K666="","",CONCATENATE("/R",K666)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G1/R1</v>
       </c>
       <c r="M666" t="s">
@@ -19466,7 +19466,7 @@
         <v>2</v>
       </c>
       <c r="L667" t="str">
-        <f>CONCATENATE(IF(A667="","",CONCATENATE("C", A667)),IF(B667="","",CONCATENATE("/G",B667)),IF(C667="","",CONCATENATE("/R",C667)), IF(D667="","",CONCATENATE("/G",B667,".",D667)), IF(E667="","",CONCATENATE("/R",E667)), IF(F667="","",CONCATENATE("/G",B667,".",D667,".",F667)), IF(G667="","",CONCATENATE("/R",G667)), IF(H667="","",CONCATENATE("/G",B667,".",D667,".",F667,".",H667)), IF(I667="","",CONCATENATE("/R",I667)),IF(J667="","",CONCATENATE("/G",B667,".",D667,".",F667,".",H667, ".",J667)), IF(K667="","",CONCATENATE("/R",K667)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2</v>
       </c>
       <c r="M667" t="s">
@@ -19487,7 +19487,7 @@
         <v>1</v>
       </c>
       <c r="L668" t="str">
-        <f>CONCATENATE(IF(A668="","",CONCATENATE("C", A668)),IF(B668="","",CONCATENATE("/G",B668)),IF(C668="","",CONCATENATE("/R",C668)), IF(D668="","",CONCATENATE("/G",B668,".",D668)), IF(E668="","",CONCATENATE("/R",E668)), IF(F668="","",CONCATENATE("/G",B668,".",D668,".",F668)), IF(G668="","",CONCATENATE("/R",G668)), IF(H668="","",CONCATENATE("/G",B668,".",D668,".",F668,".",H668)), IF(I668="","",CONCATENATE("/R",I668)),IF(J668="","",CONCATENATE("/G",B668,".",D668,".",F668,".",H668, ".",J668)), IF(K668="","",CONCATENATE("/R",K668)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2/R1</v>
       </c>
       <c r="M668" t="s">
@@ -19511,7 +19511,7 @@
         <v>1</v>
       </c>
       <c r="L669" t="str">
-        <f>CONCATENATE(IF(A669="","",CONCATENATE("C", A669)),IF(B669="","",CONCATENATE("/G",B669)),IF(C669="","",CONCATENATE("/R",C669)), IF(D669="","",CONCATENATE("/G",B669,".",D669)), IF(E669="","",CONCATENATE("/R",E669)), IF(F669="","",CONCATENATE("/G",B669,".",D669,".",F669)), IF(G669="","",CONCATENATE("/R",G669)), IF(H669="","",CONCATENATE("/G",B669,".",D669,".",F669,".",H669)), IF(I669="","",CONCATENATE("/R",I669)),IF(J669="","",CONCATENATE("/G",B669,".",D669,".",F669,".",H669, ".",J669)), IF(K669="","",CONCATENATE("/R",K669)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2/G2.1</v>
       </c>
       <c r="M669" t="s">
@@ -19538,7 +19538,7 @@
         <v>1</v>
       </c>
       <c r="L670" t="str">
-        <f>CONCATENATE(IF(A670="","",CONCATENATE("C", A670)),IF(B670="","",CONCATENATE("/G",B670)),IF(C670="","",CONCATENATE("/R",C670)), IF(D670="","",CONCATENATE("/G",B670,".",D670)), IF(E670="","",CONCATENATE("/R",E670)), IF(F670="","",CONCATENATE("/G",B670,".",D670,".",F670)), IF(G670="","",CONCATENATE("/R",G670)), IF(H670="","",CONCATENATE("/G",B670,".",D670,".",F670,".",H670)), IF(I670="","",CONCATENATE("/R",I670)),IF(J670="","",CONCATENATE("/G",B670,".",D670,".",F670,".",H670, ".",J670)), IF(K670="","",CONCATENATE("/R",K670)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2/G2.1/R1</v>
       </c>
       <c r="M670" t="s">
@@ -19565,7 +19565,7 @@
         <v>2</v>
       </c>
       <c r="L671" t="str">
-        <f>CONCATENATE(IF(A671="","",CONCATENATE("C", A671)),IF(B671="","",CONCATENATE("/G",B671)),IF(C671="","",CONCATENATE("/R",C671)), IF(D671="","",CONCATENATE("/G",B671,".",D671)), IF(E671="","",CONCATENATE("/R",E671)), IF(F671="","",CONCATENATE("/G",B671,".",D671,".",F671)), IF(G671="","",CONCATENATE("/R",G671)), IF(H671="","",CONCATENATE("/G",B671,".",D671,".",F671,".",H671)), IF(I671="","",CONCATENATE("/R",I671)),IF(J671="","",CONCATENATE("/G",B671,".",D671,".",F671,".",H671, ".",J671)), IF(K671="","",CONCATENATE("/R",K671)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2/G2.1/R2</v>
       </c>
       <c r="M671" t="s">
@@ -19592,7 +19592,7 @@
         <v>3</v>
       </c>
       <c r="L672" s="6" t="str">
-        <f>CONCATENATE(IF(A672="","",CONCATENATE("C", A672)),IF(B672="","",CONCATENATE("/G",B672)),IF(C672="","",CONCATENATE("/R",C672)), IF(D672="","",CONCATENATE("/G",B672,".",D672)), IF(E672="","",CONCATENATE("/R",E672)), IF(F672="","",CONCATENATE("/G",B672,".",D672,".",F672)), IF(G672="","",CONCATENATE("/R",G672)), IF(H672="","",CONCATENATE("/G",B672,".",D672,".",F672,".",H672)), IF(I672="","",CONCATENATE("/R",I672)),IF(J672="","",CONCATENATE("/G",B672,".",D672,".",F672,".",H672, ".",J672)), IF(K672="","",CONCATENATE("/R",K672)))</f>
+        <f t="shared" si="17"/>
         <v>C46/G2/G2.1/R3</v>
       </c>
       <c r="M672" s="6" t="s">
@@ -19610,7 +19610,7 @@
         <v>47</v>
       </c>
       <c r="L673" s="8" t="str">
-        <f>CONCATENATE(IF(A673="","",CONCATENATE("C", A673)),IF(B673="","",CONCATENATE("/G",B673)),IF(C673="","",CONCATENATE("/R",C673)), IF(D673="","",CONCATENATE("/G",B673,".",D673)), IF(E673="","",CONCATENATE("/R",E673)), IF(F673="","",CONCATENATE("/G",B673,".",D673,".",F673)), IF(G673="","",CONCATENATE("/R",G673)), IF(H673="","",CONCATENATE("/G",B673,".",D673,".",F673,".",H673)), IF(I673="","",CONCATENATE("/R",I673)),IF(J673="","",CONCATENATE("/G",B673,".",D673,".",F673,".",H673, ".",J673)), IF(K673="","",CONCATENATE("/R",K673)))</f>
+        <f t="shared" si="17"/>
         <v>C47</v>
       </c>
       <c r="M673" s="8" t="s">
@@ -19632,7 +19632,7 @@
         <v>1</v>
       </c>
       <c r="L674" t="str">
-        <f>CONCATENATE(IF(A674="","",CONCATENATE("C", A674)),IF(B674="","",CONCATENATE("/G",B674)),IF(C674="","",CONCATENATE("/R",C674)), IF(D674="","",CONCATENATE("/G",B674,".",D674)), IF(E674="","",CONCATENATE("/R",E674)), IF(F674="","",CONCATENATE("/G",B674,".",D674,".",F674)), IF(G674="","",CONCATENATE("/R",G674)), IF(H674="","",CONCATENATE("/G",B674,".",D674,".",F674,".",H674)), IF(I674="","",CONCATENATE("/R",I674)),IF(J674="","",CONCATENATE("/G",B674,".",D674,".",F674,".",H674, ".",J674)), IF(K674="","",CONCATENATE("/R",K674)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G1</v>
       </c>
       <c r="M674" t="s">
@@ -19653,7 +19653,7 @@
         <v>1</v>
       </c>
       <c r="L675" t="str">
-        <f>CONCATENATE(IF(A675="","",CONCATENATE("C", A675)),IF(B675="","",CONCATENATE("/G",B675)),IF(C675="","",CONCATENATE("/R",C675)), IF(D675="","",CONCATENATE("/G",B675,".",D675)), IF(E675="","",CONCATENATE("/R",E675)), IF(F675="","",CONCATENATE("/G",B675,".",D675,".",F675)), IF(G675="","",CONCATENATE("/R",G675)), IF(H675="","",CONCATENATE("/G",B675,".",D675,".",F675,".",H675)), IF(I675="","",CONCATENATE("/R",I675)),IF(J675="","",CONCATENATE("/G",B675,".",D675,".",F675,".",H675, ".",J675)), IF(K675="","",CONCATENATE("/R",K675)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G1/R1</v>
       </c>
       <c r="M675" t="s">
@@ -19674,7 +19674,7 @@
         <v>2</v>
       </c>
       <c r="L676" t="str">
-        <f>CONCATENATE(IF(A676="","",CONCATENATE("C", A676)),IF(B676="","",CONCATENATE("/G",B676)),IF(C676="","",CONCATENATE("/R",C676)), IF(D676="","",CONCATENATE("/G",B676,".",D676)), IF(E676="","",CONCATENATE("/R",E676)), IF(F676="","",CONCATENATE("/G",B676,".",D676,".",F676)), IF(G676="","",CONCATENATE("/R",G676)), IF(H676="","",CONCATENATE("/G",B676,".",D676,".",F676,".",H676)), IF(I676="","",CONCATENATE("/R",I676)),IF(J676="","",CONCATENATE("/G",B676,".",D676,".",F676,".",H676, ".",J676)), IF(K676="","",CONCATENATE("/R",K676)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2</v>
       </c>
       <c r="M676" t="s">
@@ -19695,7 +19695,7 @@
         <v>1</v>
       </c>
       <c r="L677" t="str">
-        <f>CONCATENATE(IF(A677="","",CONCATENATE("C", A677)),IF(B677="","",CONCATENATE("/G",B677)),IF(C677="","",CONCATENATE("/R",C677)), IF(D677="","",CONCATENATE("/G",B677,".",D677)), IF(E677="","",CONCATENATE("/R",E677)), IF(F677="","",CONCATENATE("/G",B677,".",D677,".",F677)), IF(G677="","",CONCATENATE("/R",G677)), IF(H677="","",CONCATENATE("/G",B677,".",D677,".",F677,".",H677)), IF(I677="","",CONCATENATE("/R",I677)),IF(J677="","",CONCATENATE("/G",B677,".",D677,".",F677,".",H677, ".",J677)), IF(K677="","",CONCATENATE("/R",K677)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2/R1</v>
       </c>
       <c r="M677" t="s">
@@ -19719,7 +19719,7 @@
         <v>1</v>
       </c>
       <c r="L678" t="str">
-        <f>CONCATENATE(IF(A678="","",CONCATENATE("C", A678)),IF(B678="","",CONCATENATE("/G",B678)),IF(C678="","",CONCATENATE("/R",C678)), IF(D678="","",CONCATENATE("/G",B678,".",D678)), IF(E678="","",CONCATENATE("/R",E678)), IF(F678="","",CONCATENATE("/G",B678,".",D678,".",F678)), IF(G678="","",CONCATENATE("/R",G678)), IF(H678="","",CONCATENATE("/G",B678,".",D678,".",F678,".",H678)), IF(I678="","",CONCATENATE("/R",I678)),IF(J678="","",CONCATENATE("/G",B678,".",D678,".",F678,".",H678, ".",J678)), IF(K678="","",CONCATENATE("/R",K678)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2/G2.1</v>
       </c>
       <c r="M678" t="s">
@@ -19746,7 +19746,7 @@
         <v>1</v>
       </c>
       <c r="L679" t="str">
-        <f>CONCATENATE(IF(A679="","",CONCATENATE("C", A679)),IF(B679="","",CONCATENATE("/G",B679)),IF(C679="","",CONCATENATE("/R",C679)), IF(D679="","",CONCATENATE("/G",B679,".",D679)), IF(E679="","",CONCATENATE("/R",E679)), IF(F679="","",CONCATENATE("/G",B679,".",D679,".",F679)), IF(G679="","",CONCATENATE("/R",G679)), IF(H679="","",CONCATENATE("/G",B679,".",D679,".",F679,".",H679)), IF(I679="","",CONCATENATE("/R",I679)),IF(J679="","",CONCATENATE("/G",B679,".",D679,".",F679,".",H679, ".",J679)), IF(K679="","",CONCATENATE("/R",K679)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2/G2.1/R1</v>
       </c>
       <c r="M679" t="s">
@@ -19773,7 +19773,7 @@
         <v>2</v>
       </c>
       <c r="L680" t="str">
-        <f>CONCATENATE(IF(A680="","",CONCATENATE("C", A680)),IF(B680="","",CONCATENATE("/G",B680)),IF(C680="","",CONCATENATE("/R",C680)), IF(D680="","",CONCATENATE("/G",B680,".",D680)), IF(E680="","",CONCATENATE("/R",E680)), IF(F680="","",CONCATENATE("/G",B680,".",D680,".",F680)), IF(G680="","",CONCATENATE("/R",G680)), IF(H680="","",CONCATENATE("/G",B680,".",D680,".",F680,".",H680)), IF(I680="","",CONCATENATE("/R",I680)),IF(J680="","",CONCATENATE("/G",B680,".",D680,".",F680,".",H680, ".",J680)), IF(K680="","",CONCATENATE("/R",K680)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2/G2.1/R2</v>
       </c>
       <c r="M680" t="s">
@@ -19800,7 +19800,7 @@
         <v>3</v>
       </c>
       <c r="L681" s="6" t="str">
-        <f>CONCATENATE(IF(A681="","",CONCATENATE("C", A681)),IF(B681="","",CONCATENATE("/G",B681)),IF(C681="","",CONCATENATE("/R",C681)), IF(D681="","",CONCATENATE("/G",B681,".",D681)), IF(E681="","",CONCATENATE("/R",E681)), IF(F681="","",CONCATENATE("/G",B681,".",D681,".",F681)), IF(G681="","",CONCATENATE("/R",G681)), IF(H681="","",CONCATENATE("/G",B681,".",D681,".",F681,".",H681)), IF(I681="","",CONCATENATE("/R",I681)),IF(J681="","",CONCATENATE("/G",B681,".",D681,".",F681,".",H681, ".",J681)), IF(K681="","",CONCATENATE("/R",K681)))</f>
+        <f t="shared" si="17"/>
         <v>C47/G2/G2.1/R3</v>
       </c>
       <c r="M681" s="6" t="s">
@@ -19818,7 +19818,7 @@
         <v>48</v>
       </c>
       <c r="L682" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C48</v>
       </c>
       <c r="M682" s="8" t="s">
@@ -19840,7 +19840,7 @@
         <v>1</v>
       </c>
       <c r="L683" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C48/G1</v>
       </c>
       <c r="M683" t="s">
@@ -19861,7 +19861,7 @@
         <v>1</v>
       </c>
       <c r="L684" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C48/G1/R1</v>
       </c>
       <c r="M684" t="s">
@@ -19879,7 +19879,7 @@
         <v>49</v>
       </c>
       <c r="L685" s="8" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49</v>
       </c>
       <c r="M685" s="8" t="s">
@@ -19901,7 +19901,7 @@
         <v>1</v>
       </c>
       <c r="L686" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G1</v>
       </c>
       <c r="M686" t="s">
@@ -19925,7 +19925,7 @@
         <v>1</v>
       </c>
       <c r="L687" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G1/R1</v>
       </c>
       <c r="M687" t="s">
@@ -19949,7 +19949,7 @@
         <v>2</v>
       </c>
       <c r="L688" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G1/R2</v>
       </c>
       <c r="M688" t="s">
@@ -19970,7 +19970,7 @@
         <v>2</v>
       </c>
       <c r="L689" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G2</v>
       </c>
       <c r="M689" s="13" t="s">
@@ -19994,7 +19994,7 @@
         <v>1</v>
       </c>
       <c r="L690" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G2/R1</v>
       </c>
       <c r="M690" s="13" t="s">
@@ -20021,7 +20021,7 @@
         <v>2</v>
       </c>
       <c r="L691" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G2/R2</v>
       </c>
       <c r="M691" s="13" t="s">
@@ -20045,7 +20045,7 @@
         <v>3</v>
       </c>
       <c r="L692" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G3</v>
       </c>
       <c r="M692" s="13" t="s">
@@ -20069,7 +20069,7 @@
         <v>1</v>
       </c>
       <c r="L693" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G3/R1</v>
       </c>
       <c r="M693" s="13" t="s">
@@ -20096,7 +20096,7 @@
         <v>2</v>
       </c>
       <c r="L694" s="13" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G3/R2</v>
       </c>
       <c r="M694" s="13" t="s">
@@ -20120,7 +20120,7 @@
         <v>2</v>
       </c>
       <c r="L695" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G2</v>
       </c>
       <c r="M695" t="s">
@@ -20141,7 +20141,7 @@
         <v>1</v>
       </c>
       <c r="L696" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>C49/G2/R1</v>
       </c>
       <c r="M696" t="s">
@@ -20165,7 +20165,7 @@
         <v>1</v>
       </c>
       <c r="L697" t="str">
-        <f t="shared" ref="L697:L759" si="16">CONCATENATE(IF(A697="","",CONCATENATE("C", A697)),IF(B697="","",CONCATENATE("/G",B697)),IF(C697="","",CONCATENATE("/R",C697)), IF(D697="","",CONCATENATE("/G",B697,".",D697)), IF(E697="","",CONCATENATE("/R",E697)), IF(F697="","",CONCATENATE("/G",B697,".",D697,".",F697)), IF(G697="","",CONCATENATE("/R",G697)), IF(H697="","",CONCATENATE("/G",B697,".",D697,".",F697,".",H697)), IF(I697="","",CONCATENATE("/R",I697)),IF(J697="","",CONCATENATE("/G",B697,".",D697,".",F697,".",H697, ".",J697)), IF(K697="","",CONCATENATE("/R",K697)))</f>
+        <f t="shared" ref="L697:L749" si="18">CONCATENATE(IF(A697="","",CONCATENATE("C", A697)),IF(B697="","",CONCATENATE("/G",B697)),IF(C697="","",CONCATENATE("/R",C697)), IF(D697="","",CONCATENATE("/G",B697,".",D697)), IF(E697="","",CONCATENATE("/R",E697)), IF(F697="","",CONCATENATE("/G",B697,".",D697,".",F697)), IF(G697="","",CONCATENATE("/R",G697)), IF(H697="","",CONCATENATE("/G",B697,".",D697,".",F697,".",H697)), IF(I697="","",CONCATENATE("/R",I697)),IF(J697="","",CONCATENATE("/G",B697,".",D697,".",F697,".",H697, ".",J697)), IF(K697="","",CONCATENATE("/R",K697)))</f>
         <v>C49/G2/G2.1</v>
       </c>
       <c r="M697" t="s">
@@ -20192,7 +20192,7 @@
         <v>1</v>
       </c>
       <c r="L698" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C49/G2/G2.1/R1</v>
       </c>
       <c r="M698" t="s">
@@ -20219,7 +20219,7 @@
         <v>2</v>
       </c>
       <c r="L699" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C49/G2/G2.1/R2</v>
       </c>
       <c r="M699" t="s">
@@ -20246,7 +20246,7 @@
         <v>3</v>
       </c>
       <c r="L700" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C49/G2/G2.1/R3</v>
       </c>
       <c r="M700" s="6" t="s">
@@ -20264,7 +20264,7 @@
         <v>50</v>
       </c>
       <c r="L701" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50</v>
       </c>
       <c r="M701" s="8" t="s">
@@ -20286,7 +20286,7 @@
         <v>1</v>
       </c>
       <c r="L702" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G1</v>
       </c>
       <c r="M702" t="s">
@@ -20310,7 +20310,7 @@
         <v>1</v>
       </c>
       <c r="L703" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G1/R1</v>
       </c>
       <c r="M703" t="s">
@@ -20334,7 +20334,7 @@
         <v>2</v>
       </c>
       <c r="L704" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G1/R2</v>
       </c>
       <c r="M704" t="s">
@@ -20355,7 +20355,7 @@
         <v>2</v>
       </c>
       <c r="L705" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2</v>
       </c>
       <c r="M705" s="13" t="s">
@@ -20379,7 +20379,7 @@
         <v>1</v>
       </c>
       <c r="L706" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/R1</v>
       </c>
       <c r="M706" s="13" t="s">
@@ -20406,7 +20406,7 @@
         <v>2</v>
       </c>
       <c r="L707" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/R2</v>
       </c>
       <c r="M707" s="13" t="s">
@@ -20430,7 +20430,7 @@
         <v>3</v>
       </c>
       <c r="L708" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G3</v>
       </c>
       <c r="M708" s="13" t="s">
@@ -20454,7 +20454,7 @@
         <v>1</v>
       </c>
       <c r="L709" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G3/R1</v>
       </c>
       <c r="M709" s="13" t="s">
@@ -20481,7 +20481,7 @@
         <v>2</v>
       </c>
       <c r="L710" s="13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G3/R2</v>
       </c>
       <c r="M710" s="13" t="s">
@@ -20505,7 +20505,7 @@
         <v>2</v>
       </c>
       <c r="L711" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2</v>
       </c>
       <c r="M711" t="s">
@@ -20526,7 +20526,7 @@
         <v>1</v>
       </c>
       <c r="L712" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/R1</v>
       </c>
       <c r="M712" t="s">
@@ -20550,7 +20550,7 @@
         <v>1</v>
       </c>
       <c r="L713" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/G2.1</v>
       </c>
       <c r="M713" t="s">
@@ -20577,7 +20577,7 @@
         <v>1</v>
       </c>
       <c r="L714" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/G2.1/R1</v>
       </c>
       <c r="M714" t="s">
@@ -20604,7 +20604,7 @@
         <v>2</v>
       </c>
       <c r="L715" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/G2.1/R2</v>
       </c>
       <c r="M715" t="s">
@@ -20631,7 +20631,7 @@
         <v>3</v>
       </c>
       <c r="L716" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C50/G2/G2.1/R3</v>
       </c>
       <c r="M716" s="6" t="s">
@@ -20649,7 +20649,7 @@
         <v>51</v>
       </c>
       <c r="L717" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C51</v>
       </c>
       <c r="M717" s="8" t="s">
@@ -20671,7 +20671,7 @@
         <v>1</v>
       </c>
       <c r="L718" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C51/G1</v>
       </c>
       <c r="M718" t="s">
@@ -20692,7 +20692,7 @@
         <v>1</v>
       </c>
       <c r="L719" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C51/G1/R1</v>
       </c>
       <c r="M719" t="s">
@@ -20710,7 +20710,7 @@
         <v>52</v>
       </c>
       <c r="L720" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52</v>
       </c>
       <c r="M720" s="8" t="s">
@@ -20732,7 +20732,7 @@
         <v>1</v>
       </c>
       <c r="L721" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G1</v>
       </c>
       <c r="M721" t="s">
@@ -20753,7 +20753,7 @@
         <v>1</v>
       </c>
       <c r="L722" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G1/R1</v>
       </c>
       <c r="M722" t="s">
@@ -20774,7 +20774,7 @@
         <v>2</v>
       </c>
       <c r="L723" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2</v>
       </c>
       <c r="M723" t="s">
@@ -20795,7 +20795,7 @@
         <v>1</v>
       </c>
       <c r="L724" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2/R1</v>
       </c>
       <c r="M724" t="s">
@@ -20819,7 +20819,7 @@
         <v>1</v>
       </c>
       <c r="L725" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2/G2.1</v>
       </c>
       <c r="M725" t="s">
@@ -20846,7 +20846,7 @@
         <v>1</v>
       </c>
       <c r="L726" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2/G2.1/R1</v>
       </c>
       <c r="M726" t="s">
@@ -20873,7 +20873,7 @@
         <v>2</v>
       </c>
       <c r="L727" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2/G2.1/R2</v>
       </c>
       <c r="M727" t="s">
@@ -20900,7 +20900,7 @@
         <v>3</v>
       </c>
       <c r="L728" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C52/G2/G2.1/R3</v>
       </c>
       <c r="M728" s="6" t="s">
@@ -20918,7 +20918,7 @@
         <v>53</v>
       </c>
       <c r="L729" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53</v>
       </c>
       <c r="M729" s="8" t="s">
@@ -20940,7 +20940,7 @@
         <v>1</v>
       </c>
       <c r="L730" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G1</v>
       </c>
       <c r="M730" t="s">
@@ -20961,7 +20961,7 @@
         <v>1</v>
       </c>
       <c r="L731" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G1/R1</v>
       </c>
       <c r="M731" t="s">
@@ -20982,7 +20982,7 @@
         <v>2</v>
       </c>
       <c r="L732" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2</v>
       </c>
       <c r="M732" t="s">
@@ -21003,7 +21003,7 @@
         <v>1</v>
       </c>
       <c r="L733" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2/R1</v>
       </c>
       <c r="M733" t="s">
@@ -21027,7 +21027,7 @@
         <v>1</v>
       </c>
       <c r="L734" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2/G2.1</v>
       </c>
       <c r="M734" t="s">
@@ -21054,7 +21054,7 @@
         <v>1</v>
       </c>
       <c r="L735" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2/G2.1/R1</v>
       </c>
       <c r="M735" t="s">
@@ -21081,7 +21081,7 @@
         <v>2</v>
       </c>
       <c r="L736" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2/G2.1/R2</v>
       </c>
       <c r="M736" t="s">
@@ -21108,7 +21108,7 @@
         <v>3</v>
       </c>
       <c r="L737" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C53/G2/G2.1/R3</v>
       </c>
       <c r="M737" s="6" t="s">
@@ -21126,7 +21126,7 @@
         <v>54</v>
       </c>
       <c r="L738" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54</v>
       </c>
       <c r="M738" s="8" t="s">
@@ -21148,7 +21148,7 @@
         <v>1</v>
       </c>
       <c r="L739" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G1</v>
       </c>
       <c r="M739" t="s">
@@ -21170,7 +21170,7 @@
         <v>1</v>
       </c>
       <c r="L740" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G1/R1</v>
       </c>
       <c r="M740" t="s">
@@ -21197,7 +21197,7 @@
         <v>1</v>
       </c>
       <c r="L741" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G1/G1.1</v>
       </c>
       <c r="M741" s="6" t="s">
@@ -21227,7 +21227,7 @@
         <v>1</v>
       </c>
       <c r="L742" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G1/G1.1/R1</v>
       </c>
       <c r="M742" s="6" t="s">
@@ -21251,7 +21251,7 @@
         <v>2</v>
       </c>
       <c r="L743" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2</v>
       </c>
       <c r="M743" t="s">
@@ -21272,7 +21272,7 @@
         <v>1</v>
       </c>
       <c r="L744" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2/R1</v>
       </c>
       <c r="M744" t="s">
@@ -21296,7 +21296,7 @@
         <v>1</v>
       </c>
       <c r="L745" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2/G2.1</v>
       </c>
       <c r="M745" t="s">
@@ -21323,7 +21323,7 @@
         <v>1</v>
       </c>
       <c r="L746" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2/G2.1/R1</v>
       </c>
       <c r="M746" t="s">
@@ -21350,7 +21350,7 @@
         <v>2</v>
       </c>
       <c r="L747" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2/G2.1/R2</v>
       </c>
       <c r="M747" t="s">
@@ -21377,7 +21377,7 @@
         <v>3</v>
       </c>
       <c r="L748" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C54/G2/G2.1/R3</v>
       </c>
       <c r="M748" s="6" t="s">
@@ -21395,7 +21395,7 @@
         <v>55</v>
       </c>
       <c r="L749" s="8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>C55</v>
       </c>
       <c r="M749" s="8" t="s">
@@ -21417,7 +21417,7 @@
         <v>1</v>
       </c>
       <c r="L750" t="str">
-        <f t="shared" ref="L750:L759" si="17">CONCATENATE(IF(A750="","",CONCATENATE("C", A750)),IF(B750="","",CONCATENATE("/G",B750)),IF(C750="","",CONCATENATE("/R",C750)), IF(D750="","",CONCATENATE("/G",B750,".",D750)), IF(E750="","",CONCATENATE("/R",E750)), IF(F750="","",CONCATENATE("/G",B750,".",D750,".",F750)), IF(G750="","",CONCATENATE("/R",G750)), IF(H750="","",CONCATENATE("/G",B750,".",D750,".",F750,".",H750)), IF(I750="","",CONCATENATE("/R",I750)),IF(J750="","",CONCATENATE("/G",B750,".",D750,".",F750,".",H750, ".",J750)), IF(K750="","",CONCATENATE("/R",K750)))</f>
+        <f t="shared" ref="L750:L759" si="19">CONCATENATE(IF(A750="","",CONCATENATE("C", A750)),IF(B750="","",CONCATENATE("/G",B750)),IF(C750="","",CONCATENATE("/R",C750)), IF(D750="","",CONCATENATE("/G",B750,".",D750)), IF(E750="","",CONCATENATE("/R",E750)), IF(F750="","",CONCATENATE("/G",B750,".",D750,".",F750)), IF(G750="","",CONCATENATE("/R",G750)), IF(H750="","",CONCATENATE("/G",B750,".",D750,".",F750,".",H750)), IF(I750="","",CONCATENATE("/R",I750)),IF(J750="","",CONCATENATE("/G",B750,".",D750,".",F750,".",H750, ".",J750)), IF(K750="","",CONCATENATE("/R",K750)))</f>
         <v>C55/G1</v>
       </c>
       <c r="M750" t="s">
@@ -21438,7 +21438,7 @@
         <v>1</v>
       </c>
       <c r="L751" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G1/R1</v>
       </c>
       <c r="M751" t="s">
@@ -21470,7 +21470,7 @@
       <c r="J752" s="6"/>
       <c r="K752" s="6"/>
       <c r="L752" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G1/G1.1</v>
       </c>
       <c r="M752" t="s">
@@ -21504,7 +21504,7 @@
       <c r="J753" s="6"/>
       <c r="K753" s="6"/>
       <c r="L753" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G1/G1.1/R1</v>
       </c>
       <c r="M753" t="s">
@@ -21525,7 +21525,7 @@
         <v>2</v>
       </c>
       <c r="L754" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2</v>
       </c>
       <c r="M754" t="s">
@@ -21546,7 +21546,7 @@
         <v>1</v>
       </c>
       <c r="L755" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2/R1</v>
       </c>
       <c r="M755" t="s">
@@ -21570,7 +21570,7 @@
         <v>1</v>
       </c>
       <c r="L756" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2/G2.1</v>
       </c>
       <c r="M756" t="s">
@@ -21597,7 +21597,7 @@
         <v>1</v>
       </c>
       <c r="L757" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2/G2.1/R1</v>
       </c>
       <c r="M757" t="s">
@@ -21624,7 +21624,7 @@
         <v>2</v>
       </c>
       <c r="L758" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2/G2.1/R2</v>
       </c>
       <c r="M758" t="s">
@@ -21651,7 +21651,7 @@
         <v>3</v>
       </c>
       <c r="L759" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>C55/G2/G2.1/R3</v>
       </c>
       <c r="M759" s="6" t="s">
@@ -21669,7 +21669,7 @@
         <v>56</v>
       </c>
       <c r="L760" s="8" t="str">
-        <f t="shared" ref="L757:L823" si="18">CONCATENATE(IF(A760="","",CONCATENATE("C", A760)),IF(B760="","",CONCATENATE("/G",B760)),IF(C760="","",CONCATENATE("/R",C760)), IF(D760="","",CONCATENATE("/G",B760,".",D760)), IF(E760="","",CONCATENATE("/R",E760)), IF(F760="","",CONCATENATE("/G",B760,".",D760,".",F760)), IF(G760="","",CONCATENATE("/R",G760)), IF(H760="","",CONCATENATE("/G",B760,".",D760,".",F760,".",H760)), IF(I760="","",CONCATENATE("/R",I760)),IF(J760="","",CONCATENATE("/G",B760,".",D760,".",F760,".",H760, ".",J760)), IF(K760="","",CONCATENATE("/R",K760)))</f>
+        <f t="shared" ref="L760:L823" si="20">CONCATENATE(IF(A760="","",CONCATENATE("C", A760)),IF(B760="","",CONCATENATE("/G",B760)),IF(C760="","",CONCATENATE("/R",C760)), IF(D760="","",CONCATENATE("/G",B760,".",D760)), IF(E760="","",CONCATENATE("/R",E760)), IF(F760="","",CONCATENATE("/G",B760,".",D760,".",F760)), IF(G760="","",CONCATENATE("/R",G760)), IF(H760="","",CONCATENATE("/G",B760,".",D760,".",F760,".",H760)), IF(I760="","",CONCATENATE("/R",I760)),IF(J760="","",CONCATENATE("/G",B760,".",D760,".",F760,".",H760, ".",J760)), IF(K760="","",CONCATENATE("/R",K760)))</f>
         <v>C56</v>
       </c>
       <c r="M760" s="8" t="s">
@@ -21691,7 +21691,7 @@
         <v>1</v>
       </c>
       <c r="L761" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G1</v>
       </c>
       <c r="M761" t="s">
@@ -21712,7 +21712,7 @@
         <v>1</v>
       </c>
       <c r="L762" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G1/R1</v>
       </c>
       <c r="M762" t="s">
@@ -21744,7 +21744,7 @@
       <c r="J763" s="6"/>
       <c r="K763" s="6"/>
       <c r="L763" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G1/G1.1</v>
       </c>
       <c r="M763" t="s">
@@ -21778,7 +21778,7 @@
       <c r="J764" s="6"/>
       <c r="K764" s="6"/>
       <c r="L764" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G1/G1.1/R1</v>
       </c>
       <c r="M764" t="s">
@@ -21799,7 +21799,7 @@
         <v>2</v>
       </c>
       <c r="L765" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2</v>
       </c>
       <c r="M765" t="s">
@@ -21820,7 +21820,7 @@
         <v>1</v>
       </c>
       <c r="L766" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2/R1</v>
       </c>
       <c r="M766" t="s">
@@ -21844,7 +21844,7 @@
         <v>1</v>
       </c>
       <c r="L767" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2/G2.1</v>
       </c>
       <c r="M767" t="s">
@@ -21871,7 +21871,7 @@
         <v>1</v>
       </c>
       <c r="L768" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2/G2.1/R1</v>
       </c>
       <c r="M768" t="s">
@@ -21898,7 +21898,7 @@
         <v>2</v>
       </c>
       <c r="L769" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2/G2.1/R2</v>
       </c>
       <c r="M769" t="s">
@@ -21925,7 +21925,7 @@
         <v>3</v>
       </c>
       <c r="L770" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C56/G2/G2.1/R3</v>
       </c>
       <c r="M770" s="6" t="s">
@@ -21943,7 +21943,7 @@
         <v>57</v>
       </c>
       <c r="L771" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57</v>
       </c>
       <c r="M771" s="8" t="s">
@@ -21965,7 +21965,7 @@
         <v>1</v>
       </c>
       <c r="L772" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57/G1</v>
       </c>
       <c r="M772" t="s">
@@ -21986,7 +21986,7 @@
         <v>1</v>
       </c>
       <c r="L773" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57/G1/R1</v>
       </c>
       <c r="M773" t="s">
@@ -22013,7 +22013,7 @@
         <v>1</v>
       </c>
       <c r="L774" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57/G1/G1.1</v>
       </c>
       <c r="M774" t="s">
@@ -22040,7 +22040,7 @@
         <v>1</v>
       </c>
       <c r="L775" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57/G1/G1.1/R1</v>
       </c>
       <c r="M775" t="s">
@@ -22067,7 +22067,7 @@
         <v>2</v>
       </c>
       <c r="L776" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C57/G1/G1.1/R2</v>
       </c>
       <c r="M776" t="s">
@@ -22085,7 +22085,7 @@
         <v>58</v>
       </c>
       <c r="L777" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58</v>
       </c>
       <c r="M777" s="8" t="s">
@@ -22107,7 +22107,7 @@
         <v>1</v>
       </c>
       <c r="L778" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1</v>
       </c>
       <c r="M778" s="12" t="s">
@@ -22131,7 +22131,7 @@
         <v>1</v>
       </c>
       <c r="L779" s="12" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/R1</v>
       </c>
       <c r="M779" s="12" t="s">
@@ -22155,7 +22155,7 @@
         <v>1</v>
       </c>
       <c r="L780" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1</v>
       </c>
       <c r="M780" t="s">
@@ -22206,7 +22206,7 @@
         <v>1</v>
       </c>
       <c r="L782" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1</v>
       </c>
       <c r="M782" t="s">
@@ -22236,7 +22236,7 @@
         <v>1</v>
       </c>
       <c r="L783" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1/R1</v>
       </c>
       <c r="M783" t="s">
@@ -22266,7 +22266,7 @@
         <v>2</v>
       </c>
       <c r="L784" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1/R2</v>
       </c>
       <c r="M784" t="s">
@@ -22296,7 +22296,7 @@
         <v>3</v>
       </c>
       <c r="L785" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1/R3</v>
       </c>
       <c r="M785" t="s">
@@ -22326,7 +22326,7 @@
         <v>1</v>
       </c>
       <c r="L786" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1/G1.1.1</v>
       </c>
       <c r="M786" t="s">
@@ -22356,7 +22356,7 @@
         <v>1</v>
       </c>
       <c r="L787" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.1/G1.1.1/R1</v>
       </c>
       <c r="M787" t="s">
@@ -22383,7 +22383,7 @@
         <v>2</v>
       </c>
       <c r="L788" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.2</v>
       </c>
       <c r="M788" t="s">
@@ -22413,7 +22413,7 @@
         <v>1</v>
       </c>
       <c r="L789" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.2/R1</v>
       </c>
       <c r="M789" t="s">
@@ -22443,7 +22443,7 @@
         <v>2</v>
       </c>
       <c r="L790" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C58/G1/G1.2/R2</v>
       </c>
       <c r="M790" t="s">
@@ -22464,7 +22464,7 @@
         <v>59</v>
       </c>
       <c r="L791" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59</v>
       </c>
       <c r="M791" s="8" t="s">
@@ -22486,7 +22486,7 @@
         <v>1</v>
       </c>
       <c r="L792" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1</v>
       </c>
       <c r="M792" t="s">
@@ -22507,7 +22507,7 @@
         <v>1</v>
       </c>
       <c r="L793" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1/R1</v>
       </c>
       <c r="M793" t="s">
@@ -22534,7 +22534,7 @@
         <v>1</v>
       </c>
       <c r="L794" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1/G1.1</v>
       </c>
       <c r="M794" t="s">
@@ -22561,7 +22561,7 @@
         <v>1</v>
       </c>
       <c r="L795" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1/G1.1/R1</v>
       </c>
       <c r="M795" t="s">
@@ -22588,7 +22588,7 @@
         <v>2</v>
       </c>
       <c r="L796" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1/G1.1/R2</v>
       </c>
       <c r="M796" t="s">
@@ -22615,7 +22615,7 @@
         <v>3</v>
       </c>
       <c r="L797" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C59/G1/G1.1/R3</v>
       </c>
       <c r="M797" t="s">
@@ -22633,7 +22633,7 @@
         <v>60</v>
       </c>
       <c r="L798" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C60</v>
       </c>
       <c r="M798" s="8" t="s">
@@ -22655,7 +22655,7 @@
         <v>1</v>
       </c>
       <c r="L799" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C60/G1</v>
       </c>
       <c r="M799" t="s">
@@ -22676,7 +22676,7 @@
         <v>1</v>
       </c>
       <c r="L800" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C60/G1/R1</v>
       </c>
       <c r="M800" t="s">
@@ -22697,7 +22697,7 @@
         <v>61</v>
       </c>
       <c r="L801" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C61</v>
       </c>
       <c r="M801" s="8" t="s">
@@ -22719,7 +22719,7 @@
         <v>1</v>
       </c>
       <c r="L802" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C61/G1</v>
       </c>
       <c r="M802" t="s">
@@ -22740,7 +22740,7 @@
         <v>1</v>
       </c>
       <c r="L803" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C61/G1/R1</v>
       </c>
       <c r="M803" t="s">
@@ -22764,7 +22764,7 @@
         <v>1</v>
       </c>
       <c r="L804" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C61/G1/G1.1</v>
       </c>
       <c r="M804" t="s">
@@ -22794,7 +22794,7 @@
         <v>1</v>
       </c>
       <c r="L805" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C61/G1/G1.1/R1</v>
       </c>
       <c r="M805" t="s">
@@ -22812,7 +22812,7 @@
         <v>62</v>
       </c>
       <c r="L806" s="8" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62</v>
       </c>
       <c r="M806" s="8" t="s">
@@ -22834,7 +22834,7 @@
         <v>1</v>
       </c>
       <c r="L807" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G1</v>
       </c>
       <c r="M807" t="s">
@@ -22855,7 +22855,7 @@
         <v>1</v>
       </c>
       <c r="L808" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G1/R1</v>
       </c>
       <c r="M808" t="s">
@@ -22882,7 +22882,7 @@
         <v>1</v>
       </c>
       <c r="L809" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G1/G1.1</v>
       </c>
       <c r="M809" t="s">
@@ -22909,7 +22909,7 @@
         <v>1</v>
       </c>
       <c r="L810" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G1/G1.1/R1</v>
       </c>
       <c r="M810" t="s">
@@ -22930,7 +22930,7 @@
         <v>2</v>
       </c>
       <c r="L811" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2</v>
       </c>
       <c r="M811" t="s">
@@ -22951,7 +22951,7 @@
         <v>1</v>
       </c>
       <c r="L812" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2/R1</v>
       </c>
       <c r="M812" t="s">
@@ -22975,7 +22975,7 @@
         <v>1</v>
       </c>
       <c r="L813" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2/G2.1</v>
       </c>
       <c r="M813" t="s">
@@ -23002,7 +23002,7 @@
         <v>1</v>
       </c>
       <c r="L814" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2/G2.1/R1</v>
       </c>
       <c r="M814" t="s">
@@ -23029,7 +23029,7 @@
         <v>2</v>
       </c>
       <c r="L815" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2/G2.1/R2</v>
       </c>
       <c r="M815" t="s">
@@ -23056,7 +23056,7 @@
         <v>3</v>
       </c>
       <c r="L816" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>C62/G2/G2.1/R3</v>
       </c>
       <c r="M816" s="6" t="s">
@@ -23071,43 +23071,43 @@
     </row>
     <row r="817" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L817" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="818" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L818" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="819" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L819" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="820" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L820" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="821" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L821" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="822" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L822" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="823" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L823" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Revision of the Data Structures 54-56
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomyV1.0.3_CHANGE_LOG.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomyV1.0.3_CHANGE_LOG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPD-Steps\ESPD\dist\cl\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2318,7 +2318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R823"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>